<commit_message>
Revise sample fitness calculation
</commit_message>
<xml_diff>
--- a/Excel/sample_fitness_calc.xlsx
+++ b/Excel/sample_fitness_calc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irawinder/Gits/GeneticAlgorithm/fitness_calculation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irawinder/Gits/GeneticAlgorithm/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA10AA6A-92F2-4040-B17F-1B0E22FA3AD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7901564-E713-6044-95F4-F72C53C8BD8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="3480" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24080" yWindow="3440" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -189,10 +189,10 @@
     <t>Fitness Calculation</t>
   </si>
   <si>
-    <t>Calculation</t>
-  </si>
-  <si>
     <t>(fitness)</t>
+  </si>
+  <si>
+    <t>Calculated</t>
   </si>
 </sst>
 </file>
@@ -315,6 +315,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -324,9 +327,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -612,7 +612,7 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -626,22 +626,22 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="C5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="7"/>
+      <c r="C5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -761,43 +761,43 @@
         <v>5</v>
       </c>
       <c r="C13" s="2">
-        <f>C$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C13:L13" si="0">C$8*$C37/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D13" s="2">
-        <f>D$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="E13" s="2">
-        <f>E$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="F13" s="2">
-        <f>F$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="G13" s="2">
-        <f>G$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="H13" s="2">
-        <f>H$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="I13" s="2">
-        <f>I$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="J13" s="2">
-        <f>J$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="K13" s="2">
-        <f>K$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="L13" s="2">
-        <f>L$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -806,43 +806,43 @@
         <v>6</v>
       </c>
       <c r="C14" s="2">
-        <f>C$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C14:L14" si="1">C$8*$C38/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D14" s="2">
-        <f>D$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="E14" s="2">
-        <f>E$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="F14" s="2">
-        <f>F$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="G14" s="2">
-        <f>G$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="H14" s="2">
-        <f>H$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="I14" s="2">
-        <f>I$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="J14" s="2">
-        <f>J$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="K14" s="2">
-        <f>K$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="L14" s="2">
-        <f>L$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
@@ -851,43 +851,43 @@
         <v>7</v>
       </c>
       <c r="C15" s="2">
-        <f>C$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C15:L15" si="2">C$8*$C39/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D15" s="2">
-        <f>D$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="E15" s="2">
-        <f>E$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="F15" s="2">
-        <f>F$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="G15" s="2">
-        <f>G$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="H15" s="2">
-        <f>H$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="I15" s="2">
-        <f>I$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="J15" s="2">
-        <f>J$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="K15" s="2">
-        <f>K$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="L15" s="2">
-        <f>L$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
     </row>
@@ -896,43 +896,43 @@
         <v>8</v>
       </c>
       <c r="C16" s="2">
-        <f>C$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C16:L16" si="3">C$8*$C40/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D16" s="2">
-        <f>D$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="E16" s="2">
-        <f>E$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="F16" s="2">
-        <f>F$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="G16" s="2">
-        <f>G$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="H16" s="2">
-        <f>H$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="I16" s="2">
-        <f>I$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="J16" s="2">
-        <f>J$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="K16" s="2">
-        <f>K$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="L16" s="2">
-        <f>L$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -941,43 +941,43 @@
         <v>9</v>
       </c>
       <c r="C17" s="2">
-        <f>C$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C17:L17" si="4">C$8*$C41/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D17" s="2">
-        <f>D$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="E17" s="2">
-        <f>E$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="F17" s="2">
-        <f>F$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="G17" s="2">
-        <f>G$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="H17" s="2">
-        <f>H$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="I17" s="2">
-        <f>I$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="J17" s="2">
-        <f>J$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="K17" s="2">
-        <f>K$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="L17" s="2">
-        <f>L$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -986,43 +986,43 @@
         <v>10</v>
       </c>
       <c r="C18" s="2">
-        <f>C$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C18:L18" si="5">C$8*$C42/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D18" s="2">
-        <f>D$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="E18" s="2">
-        <f>E$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="F18" s="2">
-        <f>F$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="G18" s="2">
-        <f>G$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="H18" s="2">
-        <f>H$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="I18" s="2">
-        <f>I$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="J18" s="2">
-        <f>J$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="K18" s="2">
-        <f>K$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="L18" s="2">
-        <f>L$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1031,43 +1031,43 @@
         <v>11</v>
       </c>
       <c r="C19" s="2">
-        <f>C$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C19:L19" si="6">C$8*$C43/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D19" s="2">
-        <f>D$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="E19" s="2">
-        <f>E$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="F19" s="2">
-        <f>F$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="G19" s="2">
-        <f>G$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="H19" s="2">
-        <f>H$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="I19" s="2">
-        <f>I$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="J19" s="2">
-        <f>J$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="K19" s="2">
-        <f>K$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="L19" s="2">
-        <f>L$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1076,43 +1076,43 @@
         <v>12</v>
       </c>
       <c r="C20" s="2">
-        <f>C$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C20:L20" si="7">C$8*$C44/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D20" s="2">
-        <f>D$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="E20" s="2">
-        <f>E$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="F20" s="2">
-        <f>F$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="G20" s="2">
-        <f>G$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="H20" s="2">
-        <f>H$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="I20" s="2">
-        <f>I$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="J20" s="2">
-        <f>J$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="K20" s="2">
-        <f>K$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="L20" s="2">
-        <f>L$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1121,43 +1121,43 @@
         <v>13</v>
       </c>
       <c r="C21" s="2">
-        <f>C$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C21:L21" si="8">C$8*$C45/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D21" s="2">
-        <f>D$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="E21" s="2">
-        <f>E$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="F21" s="2">
-        <f>F$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="G21" s="2">
-        <f>G$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="H21" s="2">
-        <f>H$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="I21" s="2">
-        <f>I$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="J21" s="2">
-        <f>J$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="K21" s="2">
-        <f>K$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
       <c r="L21" s="2">
-        <f>L$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" si="8"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1166,43 +1166,43 @@
         <v>14</v>
       </c>
       <c r="C22" s="2">
-        <f>C$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C22:L22" si="9">C$8*$C46/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D22" s="2">
-        <f>D$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="E22" s="2">
-        <f>E$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="F22" s="2">
-        <f>F$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="G22" s="2">
-        <f>G$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="H22" s="2">
-        <f>H$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="I22" s="2">
-        <f>I$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="J22" s="2">
-        <f>J$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="K22" s="2">
-        <f>K$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="L22" s="2">
-        <f>L$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1211,43 +1211,43 @@
         <v>15</v>
       </c>
       <c r="C23" s="2">
-        <f>C$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C23:L23" si="10">C$8*$C47/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D23" s="2">
-        <f>D$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="E23" s="2">
-        <f>E$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="F23" s="2">
-        <f>F$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="G23" s="2">
-        <f>G$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="H23" s="2">
-        <f>H$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="I23" s="2">
-        <f>I$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="J23" s="2">
-        <f>J$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="K23" s="2">
-        <f>K$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
       <c r="L23" s="2">
-        <f>L$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" si="10"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1256,43 +1256,43 @@
         <v>16</v>
       </c>
       <c r="C24" s="2">
-        <f>C$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C24:L24" si="11">C$8*$C48/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D24" s="2">
-        <f>D$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="E24" s="2">
-        <f>E$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="F24" s="2">
-        <f>F$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="G24" s="2">
-        <f>G$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="H24" s="2">
-        <f>H$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="I24" s="2">
-        <f>I$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="J24" s="2">
-        <f>J$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="K24" s="2">
-        <f>K$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="L24" s="2">
-        <f>L$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1301,43 +1301,43 @@
         <v>17</v>
       </c>
       <c r="C25" s="2">
-        <f>C$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C25:L25" si="12">C$8*$C49/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D25" s="2">
-        <f>D$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="E25" s="2">
-        <f>E$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="F25" s="2">
-        <f>F$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="G25" s="2">
-        <f>G$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="H25" s="2">
-        <f>H$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="I25" s="2">
-        <f>I$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="J25" s="2">
-        <f>J$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="K25" s="2">
-        <f>K$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="L25" s="2">
-        <f>L$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1346,43 +1346,43 @@
         <v>18</v>
       </c>
       <c r="C26" s="2">
-        <f>C$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C26:L26" si="13">C$8*$C50/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D26" s="2">
-        <f>D$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="E26" s="2">
-        <f>E$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="F26" s="2">
-        <f>F$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="G26" s="2">
-        <f>G$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="H26" s="2">
-        <f>H$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="I26" s="2">
-        <f>I$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="J26" s="2">
-        <f>J$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="K26" s="2">
-        <f>K$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="L26" s="2">
-        <f>L$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1391,43 +1391,43 @@
         <v>19</v>
       </c>
       <c r="C27" s="2">
-        <f>C$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C27:L27" si="14">C$8*$C51/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D27" s="2">
-        <f>D$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="E27" s="2">
-        <f>E$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="F27" s="2">
-        <f>F$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="G27" s="2">
-        <f>G$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="H27" s="2">
-        <f>H$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="I27" s="2">
-        <f>I$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="J27" s="2">
-        <f>J$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="K27" s="2">
-        <f>K$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
       <c r="L27" s="2">
-        <f>L$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1436,43 +1436,43 @@
         <v>20</v>
       </c>
       <c r="C28" s="2">
-        <f>C$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C28:L28" si="15">C$8*$C52/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D28" s="2">
-        <f>D$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="E28" s="2">
-        <f>E$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="F28" s="2">
-        <f>F$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="G28" s="2">
-        <f>G$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="H28" s="2">
-        <f>H$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="I28" s="2">
-        <f>I$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="J28" s="2">
-        <f>J$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="K28" s="2">
-        <f>K$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
       <c r="L28" s="2">
-        <f>L$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1481,43 +1481,43 @@
         <v>21</v>
       </c>
       <c r="C29" s="2">
-        <f>C$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C29:L29" si="16">C$8*$C53/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D29" s="2">
-        <f>D$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="E29" s="2">
-        <f>E$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="F29" s="2">
-        <f>F$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="G29" s="2">
-        <f>G$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="H29" s="2">
-        <f>H$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="I29" s="2">
-        <f>I$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="J29" s="2">
-        <f>J$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="K29" s="2">
-        <f>K$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
       <c r="L29" s="2">
-        <f>L$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" si="16"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1526,43 +1526,43 @@
         <v>22</v>
       </c>
       <c r="C30" s="2">
-        <f>C$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C30:L30" si="17">C$8*$C54/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D30" s="2">
-        <f>D$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="E30" s="2">
-        <f>E$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="F30" s="2">
-        <f>F$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="G30" s="2">
-        <f>G$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="H30" s="2">
-        <f>H$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="I30" s="2">
-        <f>I$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="J30" s="2">
-        <f>J$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="K30" s="2">
-        <f>K$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
       <c r="L30" s="2">
-        <f>L$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1571,43 +1571,43 @@
         <v>23</v>
       </c>
       <c r="C31" s="2">
-        <f>C$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C31:L31" si="18">C$8*$C55/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D31" s="2">
-        <f>D$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="E31" s="2">
-        <f>E$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="F31" s="2">
-        <f>F$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="G31" s="2">
-        <f>G$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="H31" s="2">
-        <f>H$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="I31" s="2">
-        <f>I$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="J31" s="2">
-        <f>J$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="K31" s="2">
-        <f>K$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="L31" s="2">
-        <f>L$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1616,43 +1616,43 @@
         <v>24</v>
       </c>
       <c r="C32" s="2">
-        <f>C$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C32:L32" si="19">C$8*$C56/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D32" s="2">
-        <f>D$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="E32" s="2">
-        <f>E$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="F32" s="2">
-        <f>F$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="G32" s="2">
-        <f>G$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="H32" s="2">
-        <f>H$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="I32" s="2">
-        <f>I$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="J32" s="2">
-        <f>J$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="K32" s="2">
-        <f>K$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
       <c r="L32" s="2">
-        <f>L$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" si="19"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2711,20 +2711,20 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="10"/>
-      <c r="H86" s="10"/>
-      <c r="I86" s="10"/>
-      <c r="J86" s="10"/>
-      <c r="K86" s="10"/>
-      <c r="L86" s="10"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
@@ -2762,44 +2762,44 @@
       </c>
     </row>
     <row r="89" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="C89" s="8">
+      <c r="C89" s="5">
         <f>C81*C8</f>
         <v>55</v>
       </c>
-      <c r="D89" s="8">
-        <f t="shared" ref="D89:L89" si="0">D81*D8</f>
+      <c r="D89" s="5">
+        <f t="shared" ref="D89:L89" si="20">D81*D8</f>
         <v>45</v>
       </c>
-      <c r="E89" s="8">
-        <f t="shared" si="0"/>
+      <c r="E89" s="5">
+        <f t="shared" si="20"/>
         <v>40</v>
       </c>
-      <c r="F89" s="8">
-        <f t="shared" si="0"/>
+      <c r="F89" s="5">
+        <f t="shared" si="20"/>
         <v>45</v>
       </c>
-      <c r="G89" s="8">
-        <f t="shared" si="0"/>
+      <c r="G89" s="5">
+        <f t="shared" si="20"/>
         <v>50</v>
       </c>
-      <c r="H89" s="8">
-        <f t="shared" si="0"/>
+      <c r="H89" s="5">
+        <f t="shared" si="20"/>
         <v>45</v>
       </c>
-      <c r="I89" s="8">
-        <f t="shared" si="0"/>
+      <c r="I89" s="5">
+        <f t="shared" si="20"/>
         <v>35</v>
       </c>
-      <c r="J89" s="8">
-        <f t="shared" si="0"/>
+      <c r="J89" s="5">
+        <f t="shared" si="20"/>
         <v>40</v>
       </c>
-      <c r="K89" s="8">
-        <f t="shared" si="0"/>
+      <c r="K89" s="5">
+        <f t="shared" si="20"/>
         <v>50</v>
       </c>
-      <c r="L89" s="8">
-        <f t="shared" si="0"/>
+      <c r="L89" s="5">
+        <f t="shared" si="20"/>
         <v>60</v>
       </c>
     </row>
@@ -2842,44 +2842,44 @@
       <c r="B92" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="8">
+      <c r="C92" s="5">
         <f>C59*C13</f>
         <v>3.6599999999999997</v>
       </c>
-      <c r="D92" s="8">
-        <f t="shared" ref="D92:L92" si="1">D59*D13</f>
+      <c r="D92" s="5">
+        <f t="shared" ref="D92:L92" si="21">D59*D13</f>
         <v>0.66</v>
       </c>
-      <c r="E92" s="8">
-        <f t="shared" si="1"/>
+      <c r="E92" s="5">
+        <f t="shared" si="21"/>
         <v>6.06</v>
       </c>
-      <c r="F92" s="8">
-        <f t="shared" si="1"/>
+      <c r="F92" s="5">
+        <f t="shared" si="21"/>
         <v>2.4599999999999995</v>
       </c>
-      <c r="G92" s="8">
-        <f t="shared" si="1"/>
+      <c r="G92" s="5">
+        <f t="shared" si="21"/>
         <v>3.0599999999999996</v>
       </c>
-      <c r="H92" s="8">
-        <f t="shared" si="1"/>
+      <c r="H92" s="5">
+        <f t="shared" si="21"/>
         <v>4.8599999999999994</v>
       </c>
-      <c r="I92" s="8">
-        <f t="shared" si="1"/>
+      <c r="I92" s="5">
+        <f t="shared" si="21"/>
         <v>4.26</v>
       </c>
-      <c r="J92" s="8">
-        <f t="shared" si="1"/>
+      <c r="J92" s="5">
+        <f t="shared" si="21"/>
         <v>1.8599999999999999</v>
       </c>
-      <c r="K92" s="8">
-        <f t="shared" si="1"/>
+      <c r="K92" s="5">
+        <f t="shared" si="21"/>
         <v>1.26</v>
       </c>
-      <c r="L92" s="8">
-        <f t="shared" si="1"/>
+      <c r="L92" s="5">
+        <f t="shared" si="21"/>
         <v>5.46</v>
       </c>
     </row>
@@ -2887,44 +2887,44 @@
       <c r="B93" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="8">
-        <f t="shared" ref="C93:L93" si="2">C60*C14</f>
+      <c r="C93" s="5">
+        <f t="shared" ref="C93:L93" si="22">C60*C14</f>
         <v>2.52</v>
       </c>
-      <c r="D93" s="8">
-        <f t="shared" si="2"/>
+      <c r="D93" s="5">
+        <f t="shared" si="22"/>
         <v>5.52</v>
       </c>
-      <c r="E93" s="8">
-        <f t="shared" si="2"/>
+      <c r="E93" s="5">
+        <f t="shared" si="22"/>
         <v>3.7199999999999998</v>
       </c>
-      <c r="F93" s="8">
-        <f t="shared" si="2"/>
+      <c r="F93" s="5">
+        <f t="shared" si="22"/>
         <v>6.1199999999999992</v>
       </c>
-      <c r="G93" s="8">
-        <f t="shared" si="2"/>
+      <c r="G93" s="5">
+        <f t="shared" si="22"/>
         <v>3.12</v>
       </c>
-      <c r="H93" s="8">
-        <f t="shared" si="2"/>
+      <c r="H93" s="5">
+        <f t="shared" si="22"/>
         <v>4.32</v>
       </c>
-      <c r="I93" s="8">
-        <f t="shared" si="2"/>
+      <c r="I93" s="5">
+        <f t="shared" si="22"/>
         <v>1.92</v>
       </c>
-      <c r="J93" s="8">
-        <f t="shared" si="2"/>
+      <c r="J93" s="5">
+        <f t="shared" si="22"/>
         <v>4.919999999999999</v>
       </c>
-      <c r="K93" s="8">
-        <f t="shared" si="2"/>
+      <c r="K93" s="5">
+        <f t="shared" si="22"/>
         <v>1.32</v>
       </c>
-      <c r="L93" s="8">
-        <f t="shared" si="2"/>
+      <c r="L93" s="5">
+        <f t="shared" si="22"/>
         <v>4.919999999999999</v>
       </c>
     </row>
@@ -2932,44 +2932,44 @@
       <c r="B94" t="s">
         <v>7</v>
       </c>
-      <c r="C94" s="8">
-        <f t="shared" ref="C94:L94" si="3">C61*C15</f>
+      <c r="C94" s="5">
+        <f t="shared" ref="C94:L94" si="23">C61*C15</f>
         <v>6.1800000000000006</v>
       </c>
-      <c r="D94" s="8">
-        <f t="shared" si="3"/>
+      <c r="D94" s="5">
+        <f t="shared" si="23"/>
         <v>5.58</v>
       </c>
-      <c r="E94" s="8">
-        <f t="shared" si="3"/>
+      <c r="E94" s="5">
+        <f t="shared" si="23"/>
         <v>3.78</v>
       </c>
-      <c r="F94" s="8">
-        <f t="shared" si="3"/>
+      <c r="F94" s="5">
+        <f t="shared" si="23"/>
         <v>2.5799999999999996</v>
       </c>
-      <c r="G94" s="8">
-        <f t="shared" si="3"/>
+      <c r="G94" s="5">
+        <f t="shared" si="23"/>
         <v>0.78</v>
       </c>
-      <c r="H94" s="8">
-        <f t="shared" si="3"/>
+      <c r="H94" s="5">
+        <f t="shared" si="23"/>
         <v>4.9800000000000004</v>
       </c>
-      <c r="I94" s="8">
-        <f t="shared" si="3"/>
+      <c r="I94" s="5">
+        <f t="shared" si="23"/>
         <v>4.38</v>
       </c>
-      <c r="J94" s="8">
-        <f t="shared" si="3"/>
+      <c r="J94" s="5">
+        <f t="shared" si="23"/>
         <v>1.9799999999999998</v>
       </c>
-      <c r="K94" s="8">
-        <f t="shared" si="3"/>
+      <c r="K94" s="5">
+        <f t="shared" si="23"/>
         <v>1.38</v>
       </c>
-      <c r="L94" s="8">
-        <f t="shared" si="3"/>
+      <c r="L94" s="5">
+        <f t="shared" si="23"/>
         <v>3.1799999999999997</v>
       </c>
     </row>
@@ -2977,44 +2977,44 @@
       <c r="B95" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="8">
-        <f t="shared" ref="C95:L95" si="4">C62*C16</f>
+      <c r="C95" s="5">
+        <f t="shared" ref="C95:L95" si="24">C62*C16</f>
         <v>1.44</v>
       </c>
-      <c r="D95" s="8">
-        <f t="shared" si="4"/>
+      <c r="D95" s="5">
+        <f t="shared" si="24"/>
         <v>5.64</v>
       </c>
-      <c r="E95" s="8">
-        <f t="shared" si="4"/>
+      <c r="E95" s="5">
+        <f t="shared" si="24"/>
         <v>0.84</v>
       </c>
-      <c r="F95" s="8">
-        <f t="shared" si="4"/>
+      <c r="F95" s="5">
+        <f t="shared" si="24"/>
         <v>4.4400000000000004</v>
       </c>
-      <c r="G95" s="8">
-        <f t="shared" si="4"/>
+      <c r="G95" s="5">
+        <f t="shared" si="24"/>
         <v>3.24</v>
       </c>
-      <c r="H95" s="8">
-        <f t="shared" si="4"/>
+      <c r="H95" s="5">
+        <f t="shared" si="24"/>
         <v>2.04</v>
       </c>
-      <c r="I95" s="8">
-        <f t="shared" si="4"/>
+      <c r="I95" s="5">
+        <f t="shared" si="24"/>
         <v>2.64</v>
       </c>
-      <c r="J95" s="8">
-        <f t="shared" si="4"/>
+      <c r="J95" s="5">
+        <f t="shared" si="24"/>
         <v>5.04</v>
       </c>
-      <c r="K95" s="8">
-        <f t="shared" si="4"/>
+      <c r="K95" s="5">
+        <f t="shared" si="24"/>
         <v>6.24</v>
       </c>
-      <c r="L95" s="8">
-        <f t="shared" si="4"/>
+      <c r="L95" s="5">
+        <f t="shared" si="24"/>
         <v>3.84</v>
       </c>
     </row>
@@ -3022,44 +3022,44 @@
       <c r="B96" t="s">
         <v>9</v>
       </c>
-      <c r="C96" s="8">
-        <f t="shared" ref="C96:L96" si="5">C63*C17</f>
+      <c r="C96" s="5">
+        <f t="shared" ref="C96:L96" si="25">C63*C17</f>
         <v>2.6999999999999997</v>
       </c>
-      <c r="D96" s="8">
-        <f t="shared" si="5"/>
+      <c r="D96" s="5">
+        <f t="shared" si="25"/>
         <v>3.3</v>
       </c>
-      <c r="E96" s="8">
-        <f t="shared" si="5"/>
+      <c r="E96" s="5">
+        <f t="shared" si="25"/>
         <v>3.9</v>
       </c>
-      <c r="F96" s="8">
-        <f t="shared" si="5"/>
+      <c r="F96" s="5">
+        <f t="shared" si="25"/>
         <v>6.3</v>
       </c>
-      <c r="G96" s="8">
-        <f t="shared" si="5"/>
+      <c r="G96" s="5">
+        <f t="shared" si="25"/>
         <v>5.7</v>
       </c>
-      <c r="H96" s="8">
-        <f t="shared" si="5"/>
+      <c r="H96" s="5">
+        <f t="shared" si="25"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="I96" s="8">
-        <f t="shared" si="5"/>
+      <c r="I96" s="5">
+        <f t="shared" si="25"/>
         <v>4.5</v>
       </c>
-      <c r="J96" s="8">
-        <f t="shared" si="5"/>
+      <c r="J96" s="5">
+        <f t="shared" si="25"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="K96" s="8">
-        <f t="shared" si="5"/>
+      <c r="K96" s="5">
+        <f t="shared" si="25"/>
         <v>1.5</v>
       </c>
-      <c r="L96" s="8">
-        <f t="shared" si="5"/>
+      <c r="L96" s="5">
+        <f t="shared" si="25"/>
         <v>2.1</v>
       </c>
     </row>
@@ -3067,44 +3067,44 @@
       <c r="B97" t="s">
         <v>10</v>
       </c>
-      <c r="C97" s="8">
-        <f t="shared" ref="C97:L97" si="6">C64*C18</f>
+      <c r="C97" s="5">
+        <f t="shared" ref="C97:L97" si="26">C64*C18</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D97" s="8">
-        <f t="shared" si="6"/>
+      <c r="D97" s="5">
+        <f t="shared" si="26"/>
         <v>0.96</v>
       </c>
-      <c r="E97" s="8">
-        <f t="shared" si="6"/>
+      <c r="E97" s="5">
+        <f t="shared" si="26"/>
         <v>3.9599999999999995</v>
       </c>
-      <c r="F97" s="8">
-        <f t="shared" si="6"/>
+      <c r="F97" s="5">
+        <f t="shared" si="26"/>
         <v>2.76</v>
       </c>
-      <c r="G97" s="8">
-        <f t="shared" si="6"/>
+      <c r="G97" s="5">
+        <f t="shared" si="26"/>
         <v>5.1599999999999993</v>
       </c>
-      <c r="H97" s="8">
-        <f t="shared" si="6"/>
+      <c r="H97" s="5">
+        <f t="shared" si="26"/>
         <v>2.16</v>
       </c>
-      <c r="I97" s="8">
-        <f t="shared" si="6"/>
+      <c r="I97" s="5">
+        <f t="shared" si="26"/>
         <v>4.5599999999999996</v>
       </c>
-      <c r="J97" s="8">
-        <f t="shared" si="6"/>
+      <c r="J97" s="5">
+        <f t="shared" si="26"/>
         <v>3.36</v>
       </c>
-      <c r="K97" s="8">
-        <f t="shared" si="6"/>
+      <c r="K97" s="5">
+        <f t="shared" si="26"/>
         <v>1.56</v>
       </c>
-      <c r="L97" s="8">
-        <f t="shared" si="6"/>
+      <c r="L97" s="5">
+        <f t="shared" si="26"/>
         <v>5.76</v>
       </c>
     </row>
@@ -3112,44 +3112,44 @@
       <c r="B98" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="8">
-        <f t="shared" ref="C98:L98" si="7">C65*C19</f>
+      <c r="C98" s="5">
+        <f t="shared" ref="C98:L98" si="27">C65*C19</f>
         <v>6.419999999999999</v>
       </c>
-      <c r="D98" s="8">
-        <f t="shared" si="7"/>
+      <c r="D98" s="5">
+        <f t="shared" si="27"/>
         <v>2.2200000000000002</v>
       </c>
-      <c r="E98" s="8">
-        <f t="shared" si="7"/>
+      <c r="E98" s="5">
+        <f t="shared" si="27"/>
         <v>4.0199999999999996</v>
       </c>
-      <c r="F98" s="8">
-        <f t="shared" si="7"/>
+      <c r="F98" s="5">
+        <f t="shared" si="27"/>
         <v>2.82</v>
       </c>
-      <c r="G98" s="8">
-        <f t="shared" si="7"/>
+      <c r="G98" s="5">
+        <f t="shared" si="27"/>
         <v>3.42</v>
       </c>
-      <c r="H98" s="8">
-        <f t="shared" si="7"/>
+      <c r="H98" s="5">
+        <f t="shared" si="27"/>
         <v>5.8199999999999994</v>
       </c>
-      <c r="I98" s="8">
-        <f t="shared" si="7"/>
+      <c r="I98" s="5">
+        <f t="shared" si="27"/>
         <v>1.02</v>
       </c>
-      <c r="J98" s="8">
-        <f t="shared" si="7"/>
+      <c r="J98" s="5">
+        <f t="shared" si="27"/>
         <v>5.22</v>
       </c>
-      <c r="K98" s="8">
-        <f t="shared" si="7"/>
+      <c r="K98" s="5">
+        <f t="shared" si="27"/>
         <v>1.62</v>
       </c>
-      <c r="L98" s="8">
-        <f t="shared" si="7"/>
+      <c r="L98" s="5">
+        <f t="shared" si="27"/>
         <v>4.62</v>
       </c>
     </row>
@@ -3157,44 +3157,44 @@
       <c r="B99" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="8">
-        <f t="shared" ref="C99:L99" si="8">C66*C20</f>
+      <c r="C99" s="5">
+        <f t="shared" ref="C99:L99" si="28">C66*C20</f>
         <v>6.48</v>
       </c>
-      <c r="D99" s="8">
-        <f t="shared" si="8"/>
+      <c r="D99" s="5">
+        <f t="shared" si="28"/>
         <v>5.88</v>
       </c>
-      <c r="E99" s="8">
-        <f t="shared" si="8"/>
+      <c r="E99" s="5">
+        <f t="shared" si="28"/>
         <v>4.08</v>
       </c>
-      <c r="F99" s="8">
-        <f t="shared" si="8"/>
+      <c r="F99" s="5">
+        <f t="shared" si="28"/>
         <v>2.88</v>
       </c>
-      <c r="G99" s="8">
-        <f t="shared" si="8"/>
+      <c r="G99" s="5">
+        <f t="shared" si="28"/>
         <v>3.48</v>
       </c>
-      <c r="H99" s="8">
-        <f t="shared" si="8"/>
+      <c r="H99" s="5">
+        <f t="shared" si="28"/>
         <v>1.08</v>
       </c>
-      <c r="I99" s="8">
-        <f t="shared" si="8"/>
+      <c r="I99" s="5">
+        <f t="shared" si="28"/>
         <v>4.68</v>
       </c>
-      <c r="J99" s="8">
-        <f t="shared" si="8"/>
+      <c r="J99" s="5">
+        <f t="shared" si="28"/>
         <v>1.08</v>
       </c>
-      <c r="K99" s="8">
-        <f t="shared" si="8"/>
+      <c r="K99" s="5">
+        <f t="shared" si="28"/>
         <v>1.68</v>
       </c>
-      <c r="L99" s="8">
-        <f t="shared" si="8"/>
+      <c r="L99" s="5">
+        <f t="shared" si="28"/>
         <v>5.28</v>
       </c>
     </row>
@@ -3202,44 +3202,44 @@
       <c r="B100" t="s">
         <v>13</v>
       </c>
-      <c r="C100" s="8">
-        <f t="shared" ref="C100:L100" si="9">C67*C21</f>
+      <c r="C100" s="5">
+        <f t="shared" ref="C100:L100" si="29">C67*C21</f>
         <v>6.54</v>
       </c>
-      <c r="D100" s="8">
-        <f t="shared" si="9"/>
+      <c r="D100" s="5">
+        <f t="shared" si="29"/>
         <v>5.94</v>
       </c>
-      <c r="E100" s="8">
-        <f t="shared" si="9"/>
+      <c r="E100" s="5">
+        <f t="shared" si="29"/>
         <v>4.1399999999999997</v>
       </c>
-      <c r="F100" s="8">
-        <f t="shared" si="9"/>
+      <c r="F100" s="5">
+        <f t="shared" si="29"/>
         <v>2.94</v>
       </c>
-      <c r="G100" s="8">
-        <f t="shared" si="9"/>
+      <c r="G100" s="5">
+        <f t="shared" si="29"/>
         <v>3.54</v>
       </c>
-      <c r="H100" s="8">
-        <f t="shared" si="9"/>
+      <c r="H100" s="5">
+        <f t="shared" si="29"/>
         <v>2.34</v>
       </c>
-      <c r="I100" s="8">
-        <f t="shared" si="9"/>
+      <c r="I100" s="5">
+        <f t="shared" si="29"/>
         <v>1.74</v>
       </c>
-      <c r="J100" s="8">
-        <f t="shared" si="9"/>
+      <c r="J100" s="5">
+        <f t="shared" si="29"/>
         <v>5.34</v>
       </c>
-      <c r="K100" s="8">
-        <f t="shared" si="9"/>
+      <c r="K100" s="5">
+        <f t="shared" si="29"/>
         <v>4.74</v>
       </c>
-      <c r="L100" s="8">
-        <f t="shared" si="9"/>
+      <c r="L100" s="5">
+        <f t="shared" si="29"/>
         <v>2.34</v>
       </c>
     </row>
@@ -3247,44 +3247,44 @@
       <c r="B101" t="s">
         <v>14</v>
       </c>
-      <c r="C101" s="8">
-        <f t="shared" ref="C101:L101" si="10">C68*C22</f>
+      <c r="C101" s="5">
+        <f t="shared" ref="C101:L101" si="30">C68*C22</f>
         <v>6.24</v>
       </c>
-      <c r="D101" s="8">
-        <f t="shared" si="10"/>
+      <c r="D101" s="5">
+        <f t="shared" si="30"/>
         <v>1.92</v>
       </c>
-      <c r="E101" s="8">
-        <f t="shared" si="10"/>
+      <c r="E101" s="5">
+        <f t="shared" si="30"/>
         <v>3.84</v>
       </c>
-      <c r="F101" s="8">
-        <f t="shared" si="10"/>
+      <c r="F101" s="5">
+        <f t="shared" si="30"/>
         <v>2.5799999999999996</v>
       </c>
-      <c r="G101" s="8">
-        <f t="shared" si="10"/>
+      <c r="G101" s="5">
+        <f t="shared" si="30"/>
         <v>0.78</v>
       </c>
-      <c r="H101" s="8">
-        <f t="shared" si="10"/>
+      <c r="H101" s="5">
+        <f t="shared" si="30"/>
         <v>5.28</v>
       </c>
-      <c r="I101" s="8">
-        <f t="shared" si="10"/>
+      <c r="I101" s="5">
+        <f t="shared" si="30"/>
         <v>4.1399999999999997</v>
       </c>
-      <c r="J101" s="8">
-        <f t="shared" si="10"/>
+      <c r="J101" s="5">
+        <f t="shared" si="30"/>
         <v>5.04</v>
       </c>
-      <c r="K101" s="8">
-        <f t="shared" si="10"/>
+      <c r="K101" s="5">
+        <f t="shared" si="30"/>
         <v>1.1399999999999999</v>
       </c>
-      <c r="L101" s="8">
-        <f t="shared" si="10"/>
+      <c r="L101" s="5">
+        <f t="shared" si="30"/>
         <v>3.24</v>
       </c>
     </row>
@@ -3292,44 +3292,44 @@
       <c r="B102" t="s">
         <v>15</v>
       </c>
-      <c r="C102" s="8">
-        <f t="shared" ref="C102:L102" si="11">C69*C23</f>
+      <c r="C102" s="5">
+        <f t="shared" ref="C102:L102" si="31">C69*C23</f>
         <v>1.26</v>
       </c>
-      <c r="D102" s="8">
-        <f t="shared" si="11"/>
+      <c r="D102" s="5">
+        <f t="shared" si="31"/>
         <v>5.46</v>
       </c>
-      <c r="E102" s="8">
-        <f t="shared" si="11"/>
+      <c r="E102" s="5">
+        <f t="shared" si="31"/>
         <v>2.4599999999999995</v>
       </c>
-      <c r="F102" s="8">
-        <f t="shared" si="11"/>
+      <c r="F102" s="5">
+        <f t="shared" si="31"/>
         <v>3.6599999999999997</v>
       </c>
-      <c r="G102" s="8">
-        <f t="shared" si="11"/>
+      <c r="G102" s="5">
+        <f t="shared" si="31"/>
         <v>3.0599999999999996</v>
       </c>
-      <c r="H102" s="8">
-        <f t="shared" si="11"/>
+      <c r="H102" s="5">
+        <f t="shared" si="31"/>
         <v>1.8599999999999999</v>
       </c>
-      <c r="I102" s="8">
-        <f t="shared" si="11"/>
+      <c r="I102" s="5">
+        <f t="shared" si="31"/>
         <v>4.26</v>
       </c>
-      <c r="J102" s="8">
-        <f t="shared" si="11"/>
+      <c r="J102" s="5">
+        <f t="shared" si="31"/>
         <v>0.66</v>
       </c>
-      <c r="K102" s="8">
-        <f t="shared" si="11"/>
+      <c r="K102" s="5">
+        <f t="shared" si="31"/>
         <v>6.06</v>
       </c>
-      <c r="L102" s="8">
-        <f t="shared" si="11"/>
+      <c r="L102" s="5">
+        <f t="shared" si="31"/>
         <v>4.919999999999999</v>
       </c>
     </row>
@@ -3337,44 +3337,44 @@
       <c r="B103" t="s">
         <v>16</v>
       </c>
-      <c r="C103" s="8">
-        <f t="shared" ref="C103:L103" si="12">C70*C24</f>
+      <c r="C103" s="5">
+        <f t="shared" ref="C103:L103" si="32">C70*C24</f>
         <v>6.1199999999999992</v>
       </c>
-      <c r="D103" s="8">
-        <f t="shared" si="12"/>
+      <c r="D103" s="5">
+        <f t="shared" si="32"/>
         <v>5.52</v>
       </c>
-      <c r="E103" s="8">
-        <f t="shared" si="12"/>
+      <c r="E103" s="5">
+        <f t="shared" si="32"/>
         <v>3.7199999999999998</v>
       </c>
-      <c r="F103" s="8">
-        <f t="shared" si="12"/>
+      <c r="F103" s="5">
+        <f t="shared" si="32"/>
         <v>4.919999999999999</v>
       </c>
-      <c r="G103" s="8">
-        <f t="shared" si="12"/>
+      <c r="G103" s="5">
+        <f t="shared" si="32"/>
         <v>3.12</v>
       </c>
-      <c r="H103" s="8">
-        <f t="shared" si="12"/>
+      <c r="H103" s="5">
+        <f t="shared" si="32"/>
         <v>1.92</v>
       </c>
-      <c r="I103" s="8">
-        <f t="shared" si="12"/>
+      <c r="I103" s="5">
+        <f t="shared" si="32"/>
         <v>4.32</v>
       </c>
-      <c r="J103" s="8">
-        <f t="shared" si="12"/>
+      <c r="J103" s="5">
+        <f t="shared" si="32"/>
         <v>2.52</v>
       </c>
-      <c r="K103" s="8">
-        <f t="shared" si="12"/>
+      <c r="K103" s="5">
+        <f t="shared" si="32"/>
         <v>0.72</v>
       </c>
-      <c r="L103" s="8">
-        <f t="shared" si="12"/>
+      <c r="L103" s="5">
+        <f t="shared" si="32"/>
         <v>1.26</v>
       </c>
     </row>
@@ -3382,44 +3382,44 @@
       <c r="B104" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="8">
-        <f t="shared" ref="C104:L104" si="13">C71*C25</f>
+      <c r="C104" s="5">
+        <f t="shared" ref="C104:L104" si="33">C71*C25</f>
         <v>4.38</v>
       </c>
-      <c r="D104" s="8">
-        <f t="shared" si="13"/>
+      <c r="D104" s="5">
+        <f t="shared" si="33"/>
         <v>1.9799999999999998</v>
       </c>
-      <c r="E104" s="8">
-        <f t="shared" si="13"/>
+      <c r="E104" s="5">
+        <f t="shared" si="33"/>
         <v>0.78</v>
       </c>
-      <c r="F104" s="8">
-        <f t="shared" si="13"/>
+      <c r="F104" s="5">
+        <f t="shared" si="33"/>
         <v>2.5799999999999996</v>
       </c>
-      <c r="G104" s="8">
-        <f t="shared" si="13"/>
+      <c r="G104" s="5">
+        <f t="shared" si="33"/>
         <v>3.1799999999999997</v>
       </c>
-      <c r="H104" s="8">
-        <f t="shared" si="13"/>
+      <c r="H104" s="5">
+        <f t="shared" si="33"/>
         <v>5.58</v>
       </c>
-      <c r="I104" s="8">
-        <f t="shared" si="13"/>
+      <c r="I104" s="5">
+        <f t="shared" si="33"/>
         <v>6.1800000000000006</v>
       </c>
-      <c r="J104" s="8">
-        <f t="shared" si="13"/>
+      <c r="J104" s="5">
+        <f t="shared" si="33"/>
         <v>4.9800000000000004</v>
       </c>
-      <c r="K104" s="8">
-        <f t="shared" si="13"/>
+      <c r="K104" s="5">
+        <f t="shared" si="33"/>
         <v>1.38</v>
       </c>
-      <c r="L104" s="8">
-        <f t="shared" si="13"/>
+      <c r="L104" s="5">
+        <f t="shared" si="33"/>
         <v>3.78</v>
       </c>
     </row>
@@ -3427,44 +3427,44 @@
       <c r="B105" t="s">
         <v>18</v>
       </c>
-      <c r="C105" s="8">
-        <f t="shared" ref="C105:L105" si="14">C72*C26</f>
+      <c r="C105" s="5">
+        <f t="shared" ref="C105:L105" si="34">C72*C26</f>
         <v>2.04</v>
       </c>
-      <c r="D105" s="8">
-        <f t="shared" si="14"/>
+      <c r="D105" s="5">
+        <f t="shared" si="34"/>
         <v>2.64</v>
       </c>
-      <c r="E105" s="8">
-        <f t="shared" si="14"/>
+      <c r="E105" s="5">
+        <f t="shared" si="34"/>
         <v>3.84</v>
       </c>
-      <c r="F105" s="8">
-        <f t="shared" si="14"/>
+      <c r="F105" s="5">
+        <f t="shared" si="34"/>
         <v>5.64</v>
       </c>
-      <c r="G105" s="8">
-        <f t="shared" si="14"/>
+      <c r="G105" s="5">
+        <f t="shared" si="34"/>
         <v>3.24</v>
       </c>
-      <c r="H105" s="8">
-        <f t="shared" si="14"/>
+      <c r="H105" s="5">
+        <f t="shared" si="34"/>
         <v>6.24</v>
       </c>
-      <c r="I105" s="8">
-        <f t="shared" si="14"/>
+      <c r="I105" s="5">
+        <f t="shared" si="34"/>
         <v>1.44</v>
       </c>
-      <c r="J105" s="8">
-        <f t="shared" si="14"/>
+      <c r="J105" s="5">
+        <f t="shared" si="34"/>
         <v>0.84</v>
       </c>
-      <c r="K105" s="8">
-        <f t="shared" si="14"/>
+      <c r="K105" s="5">
+        <f t="shared" si="34"/>
         <v>4.4400000000000004</v>
       </c>
-      <c r="L105" s="8">
-        <f t="shared" si="14"/>
+      <c r="L105" s="5">
+        <f t="shared" si="34"/>
         <v>5.04</v>
       </c>
     </row>
@@ -3472,44 +3472,44 @@
       <c r="B106" t="s">
         <v>19</v>
       </c>
-      <c r="C106" s="8">
-        <f t="shared" ref="C106:L106" si="15">C73*C27</f>
+      <c r="C106" s="5">
+        <f t="shared" ref="C106:L106" si="35">C73*C27</f>
         <v>3.3</v>
       </c>
-      <c r="D106" s="8">
-        <f t="shared" si="15"/>
+      <c r="D106" s="5">
+        <f t="shared" si="35"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="E106" s="8">
-        <f t="shared" si="15"/>
+      <c r="E106" s="5">
+        <f t="shared" si="35"/>
         <v>3.9</v>
       </c>
-      <c r="F106" s="8">
-        <f t="shared" si="15"/>
+      <c r="F106" s="5">
+        <f t="shared" si="35"/>
         <v>2.6999999999999997</v>
       </c>
-      <c r="G106" s="8">
-        <f t="shared" si="15"/>
+      <c r="G106" s="5">
+        <f t="shared" si="35"/>
         <v>6.3</v>
       </c>
-      <c r="H106" s="8">
-        <f t="shared" si="15"/>
+      <c r="H106" s="5">
+        <f t="shared" si="35"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="I106" s="8">
-        <f t="shared" si="15"/>
+      <c r="I106" s="5">
+        <f t="shared" si="35"/>
         <v>4.5</v>
       </c>
-      <c r="J106" s="8">
-        <f t="shared" si="15"/>
+      <c r="J106" s="5">
+        <f t="shared" si="35"/>
         <v>2.1</v>
       </c>
-      <c r="K106" s="8">
-        <f t="shared" si="15"/>
+      <c r="K106" s="5">
+        <f t="shared" si="35"/>
         <v>1.5</v>
       </c>
-      <c r="L106" s="8">
-        <f t="shared" si="15"/>
+      <c r="L106" s="5">
+        <f t="shared" si="35"/>
         <v>5.7</v>
       </c>
     </row>
@@ -3517,44 +3517,44 @@
       <c r="B107" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="8">
-        <f t="shared" ref="C107:L107" si="16">C74*C28</f>
+      <c r="C107" s="5">
+        <f t="shared" ref="C107:L107" si="36">C74*C28</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D107" s="8">
-        <f t="shared" si="16"/>
+      <c r="D107" s="5">
+        <f t="shared" si="36"/>
         <v>2.76</v>
       </c>
-      <c r="E107" s="8">
-        <f t="shared" si="16"/>
+      <c r="E107" s="5">
+        <f t="shared" si="36"/>
         <v>3.9599999999999995</v>
       </c>
-      <c r="F107" s="8">
-        <f t="shared" si="16"/>
+      <c r="F107" s="5">
+        <f t="shared" si="36"/>
         <v>3.36</v>
       </c>
-      <c r="G107" s="8">
-        <f t="shared" si="16"/>
+      <c r="G107" s="5">
+        <f t="shared" si="36"/>
         <v>5.76</v>
       </c>
-      <c r="H107" s="8">
-        <f t="shared" si="16"/>
+      <c r="H107" s="5">
+        <f t="shared" si="36"/>
         <v>5.1599999999999993</v>
       </c>
-      <c r="I107" s="8">
-        <f t="shared" si="16"/>
+      <c r="I107" s="5">
+        <f t="shared" si="36"/>
         <v>0.96</v>
       </c>
-      <c r="J107" s="8">
-        <f t="shared" si="16"/>
+      <c r="J107" s="5">
+        <f t="shared" si="36"/>
         <v>2.16</v>
       </c>
-      <c r="K107" s="8">
-        <f t="shared" si="16"/>
+      <c r="K107" s="5">
+        <f t="shared" si="36"/>
         <v>1.56</v>
       </c>
-      <c r="L107" s="8">
-        <f t="shared" si="16"/>
+      <c r="L107" s="5">
+        <f t="shared" si="36"/>
         <v>4.5599999999999996</v>
       </c>
     </row>
@@ -3562,44 +3562,44 @@
       <c r="B108" t="s">
         <v>21</v>
       </c>
-      <c r="C108" s="8">
-        <f t="shared" ref="C108:L108" si="17">C75*C29</f>
+      <c r="C108" s="5">
+        <f t="shared" ref="C108:L108" si="37">C75*C29</f>
         <v>2.2200000000000002</v>
       </c>
-      <c r="D108" s="8">
-        <f t="shared" si="17"/>
+      <c r="D108" s="5">
+        <f t="shared" si="37"/>
         <v>3.42</v>
       </c>
-      <c r="E108" s="8">
-        <f t="shared" si="17"/>
+      <c r="E108" s="5">
+        <f t="shared" si="37"/>
         <v>6.419999999999999</v>
       </c>
-      <c r="F108" s="8">
-        <f t="shared" si="17"/>
+      <c r="F108" s="5">
+        <f t="shared" si="37"/>
         <v>1.02</v>
       </c>
-      <c r="G108" s="8">
-        <f t="shared" si="17"/>
+      <c r="G108" s="5">
+        <f t="shared" si="37"/>
         <v>5.8199999999999994</v>
       </c>
-      <c r="H108" s="8">
-        <f t="shared" si="17"/>
+      <c r="H108" s="5">
+        <f t="shared" si="37"/>
         <v>4.0199999999999996</v>
       </c>
-      <c r="I108" s="8">
-        <f t="shared" si="17"/>
+      <c r="I108" s="5">
+        <f t="shared" si="37"/>
         <v>4.62</v>
       </c>
-      <c r="J108" s="8">
-        <f t="shared" si="17"/>
+      <c r="J108" s="5">
+        <f t="shared" si="37"/>
         <v>5.22</v>
       </c>
-      <c r="K108" s="8">
-        <f t="shared" si="17"/>
+      <c r="K108" s="5">
+        <f t="shared" si="37"/>
         <v>1.62</v>
       </c>
-      <c r="L108" s="8">
-        <f t="shared" si="17"/>
+      <c r="L108" s="5">
+        <f t="shared" si="37"/>
         <v>2.82</v>
       </c>
     </row>
@@ -3607,44 +3607,44 @@
       <c r="B109" t="s">
         <v>22</v>
       </c>
-      <c r="C109" s="8">
-        <f t="shared" ref="C109:L109" si="18">C76*C30</f>
+      <c r="C109" s="5">
+        <f t="shared" ref="C109:L109" si="38">C76*C30</f>
         <v>6.48</v>
       </c>
-      <c r="D109" s="8">
-        <f t="shared" si="18"/>
+      <c r="D109" s="5">
+        <f t="shared" si="38"/>
         <v>1.08</v>
       </c>
-      <c r="E109" s="8">
-        <f t="shared" si="18"/>
+      <c r="E109" s="5">
+        <f t="shared" si="38"/>
         <v>4.08</v>
       </c>
-      <c r="F109" s="8">
-        <f t="shared" si="18"/>
+      <c r="F109" s="5">
+        <f t="shared" si="38"/>
         <v>2.88</v>
       </c>
-      <c r="G109" s="8">
-        <f t="shared" si="18"/>
+      <c r="G109" s="5">
+        <f t="shared" si="38"/>
         <v>3.48</v>
       </c>
-      <c r="H109" s="8">
-        <f t="shared" si="18"/>
+      <c r="H109" s="5">
+        <f t="shared" si="38"/>
         <v>2.2799999999999998</v>
       </c>
-      <c r="I109" s="8">
-        <f t="shared" si="18"/>
+      <c r="I109" s="5">
+        <f t="shared" si="38"/>
         <v>4.68</v>
       </c>
-      <c r="J109" s="8">
-        <f t="shared" si="18"/>
+      <c r="J109" s="5">
+        <f t="shared" si="38"/>
         <v>5.28</v>
       </c>
-      <c r="K109" s="8">
-        <f t="shared" si="18"/>
+      <c r="K109" s="5">
+        <f t="shared" si="38"/>
         <v>1.68</v>
       </c>
-      <c r="L109" s="8">
-        <f t="shared" si="18"/>
+      <c r="L109" s="5">
+        <f t="shared" si="38"/>
         <v>5.88</v>
       </c>
     </row>
@@ -3652,44 +3652,44 @@
       <c r="B110" t="s">
         <v>23</v>
       </c>
-      <c r="C110" s="8">
-        <f t="shared" ref="C110:L110" si="19">C77*C31</f>
+      <c r="C110" s="5">
+        <f t="shared" ref="C110:L110" si="39">C77*C31</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="D110" s="8">
-        <f t="shared" si="19"/>
+      <c r="D110" s="5">
+        <f t="shared" si="39"/>
         <v>5.94</v>
       </c>
-      <c r="E110" s="8">
-        <f t="shared" si="19"/>
+      <c r="E110" s="5">
+        <f t="shared" si="39"/>
         <v>4.1399999999999997</v>
       </c>
-      <c r="F110" s="8">
-        <f t="shared" si="19"/>
+      <c r="F110" s="5">
+        <f t="shared" si="39"/>
         <v>2.94</v>
       </c>
-      <c r="G110" s="8">
-        <f t="shared" si="19"/>
+      <c r="G110" s="5">
+        <f t="shared" si="39"/>
         <v>3.54</v>
       </c>
-      <c r="H110" s="8">
-        <f t="shared" si="19"/>
+      <c r="H110" s="5">
+        <f t="shared" si="39"/>
         <v>4.74</v>
       </c>
-      <c r="I110" s="8">
-        <f t="shared" si="19"/>
+      <c r="I110" s="5">
+        <f t="shared" si="39"/>
         <v>2.34</v>
       </c>
-      <c r="J110" s="8">
-        <f t="shared" si="19"/>
+      <c r="J110" s="5">
+        <f t="shared" si="39"/>
         <v>5.34</v>
       </c>
-      <c r="K110" s="8">
-        <f t="shared" si="19"/>
+      <c r="K110" s="5">
+        <f t="shared" si="39"/>
         <v>1.74</v>
       </c>
-      <c r="L110" s="8">
-        <f t="shared" si="19"/>
+      <c r="L110" s="5">
+        <f t="shared" si="39"/>
         <v>6.54</v>
       </c>
     </row>
@@ -3697,44 +3697,44 @@
       <c r="B111" t="s">
         <v>24</v>
       </c>
-      <c r="C111" s="8">
-        <f t="shared" ref="C111:L111" si="20">C78*C32</f>
+      <c r="C111" s="5">
+        <f t="shared" ref="C111:L111" si="40">C78*C32</f>
         <v>1.74</v>
       </c>
-      <c r="D111" s="8">
-        <f t="shared" si="20"/>
+      <c r="D111" s="5">
+        <f t="shared" si="40"/>
         <v>3.24</v>
       </c>
-      <c r="E111" s="8">
-        <f t="shared" si="20"/>
+      <c r="E111" s="5">
+        <f t="shared" si="40"/>
         <v>5.88</v>
       </c>
-      <c r="F111" s="8">
-        <f t="shared" si="20"/>
+      <c r="F111" s="5">
+        <f t="shared" si="40"/>
         <v>3.3</v>
       </c>
-      <c r="G111" s="8">
-        <f t="shared" si="20"/>
+      <c r="G111" s="5">
+        <f t="shared" si="40"/>
         <v>2.82</v>
       </c>
-      <c r="H111" s="8">
-        <f t="shared" si="20"/>
+      <c r="H111" s="5">
+        <f t="shared" si="40"/>
         <v>1.38</v>
       </c>
-      <c r="I111" s="8">
-        <f t="shared" si="20"/>
+      <c r="I111" s="5">
+        <f t="shared" si="40"/>
         <v>3.84</v>
       </c>
-      <c r="J111" s="8">
-        <f t="shared" si="20"/>
+      <c r="J111" s="5">
+        <f t="shared" si="40"/>
         <v>4.68</v>
       </c>
-      <c r="K111" s="8">
-        <f t="shared" si="20"/>
+      <c r="K111" s="5">
+        <f t="shared" si="40"/>
         <v>2.04</v>
       </c>
-      <c r="L111" s="8">
-        <f t="shared" si="20"/>
+      <c r="L111" s="5">
+        <f t="shared" si="40"/>
         <v>2.6999999999999997</v>
       </c>
     </row>
@@ -3745,9 +3745,9 @@
     </row>
     <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>52</v>
-      </c>
-      <c r="C114" s="8">
+        <v>51</v>
+      </c>
+      <c r="C114" s="5">
         <f>SUM(C89:L89) + SUM(C92:L111)</f>
         <v>1183.02</v>
       </c>

</xml_diff>

<commit_message>
Revise Spreadsheet to include Capacity Check
</commit_message>
<xml_diff>
--- a/Excel/sample_fitness_calc.xlsx
+++ b/Excel/sample_fitness_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irawinder/Gits/GeneticAlgorithm/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7901564-E713-6044-95F4-F72C53C8BD8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2977724-DA5F-1F49-A8C0-3D9B830FC0A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24080" yWindow="3440" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17640" yWindow="3280" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="58">
   <si>
     <t>ai</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>Calculated</t>
+  </si>
+  <si>
+    <t>Valid Allocation***</t>
+  </si>
+  <si>
+    <t>*** This value must remain true to be considered as a candidate for fitness</t>
+  </si>
+  <si>
+    <t>Total Allocation</t>
+  </si>
+  <si>
+    <t>Over Capacity</t>
+  </si>
+  <si>
+    <t>(within capacity)</t>
   </si>
 </sst>
 </file>
@@ -609,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D06AB2D-3E1B-4452-B31C-A68F8850C0A4}">
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -761,7 +776,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C13:L13" si="0">C$8*$C37/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C13:L13" si="0">C$8*$C48/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D13" s="2">
@@ -806,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" ref="C14:L14" si="1">C$8*$C38/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C14:L14" si="1">C$8*$C49/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D14" s="2">
@@ -851,7 +866,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" ref="C15:L15" si="2">C$8*$C39/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C15:L15" si="2">C$8*$C50/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D15" s="2">
@@ -896,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" ref="C16:L16" si="3">C$8*$C40/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C16:L16" si="3">C$8*$C51/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D16" s="2">
@@ -941,7 +956,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" ref="C17:L17" si="4">C$8*$C41/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C17:L17" si="4">C$8*$C52/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D17" s="2">
@@ -986,7 +1001,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:L18" si="5">C$8*$C42/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C18:L18" si="5">C$8*$C53/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D18" s="2">
@@ -1031,7 +1046,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" ref="C19:L19" si="6">C$8*$C43/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C19:L19" si="6">C$8*$C54/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D19" s="2">
@@ -1076,7 +1091,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" ref="C20:L20" si="7">C$8*$C44/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C20:L20" si="7">C$8*$C55/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D20" s="2">
@@ -1121,7 +1136,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:L21" si="8">C$8*$C45/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C21:L21" si="8">C$8*$C56/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D21" s="2">
@@ -1166,7 +1181,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" ref="C22:L22" si="9">C$8*$C46/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C22:L22" si="9">C$8*$C57/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D22" s="2">
@@ -1211,7 +1226,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" ref="C23:L23" si="10">C$8*$C47/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C23:L23" si="10">C$8*$C58/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D23" s="2">
@@ -1256,7 +1271,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" ref="C24:L24" si="11">C$8*$C48/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C24:L24" si="11">C$8*$C59/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D24" s="2">
@@ -1301,7 +1316,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" ref="C25:L25" si="12">C$8*$C49/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C25:L25" si="12">C$8*$C60/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D25" s="2">
@@ -1346,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" ref="C26:L26" si="13">C$8*$C50/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C26:L26" si="13">C$8*$C61/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D26" s="2">
@@ -1391,7 +1406,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" ref="C27:L27" si="14">C$8*$C51/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C27:L27" si="14">C$8*$C62/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D27" s="2">
@@ -1436,7 +1451,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" ref="C28:L28" si="15">C$8*$C52/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C28:L28" si="15">C$8*$C63/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D28" s="2">
@@ -1481,7 +1496,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" ref="C29:L29" si="16">C$8*$C53/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C29:L29" si="16">C$8*$C64/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D29" s="2">
@@ -1526,7 +1541,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" ref="C30:L30" si="17">C$8*$C54/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C30:L30" si="17">C$8*$C65/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D30" s="2">
@@ -1571,7 +1586,7 @@
         <v>23</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" ref="C31:L31" si="18">C$8*$C55/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C31:L31" si="18">C$8*$C66/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D31" s="2">
@@ -1616,7 +1631,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" ref="C32:L32" si="19">C$8*$C56/SUM($C$8:$L$8)</f>
+        <f t="shared" ref="C32:L32" si="19">C$8*$C67/SUM($C$8:$L$8)</f>
         <v>0.6</v>
       </c>
       <c r="D32" s="2">
@@ -1656,1156 +1671,1096 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="C37" s="5">
+        <f>SUM(C13:C32)</f>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" ref="D37:L37" si="20">SUM(D13:D32)</f>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" si="20"/>
+        <v>11.999999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" t="s">
+        <v>31</v>
+      </c>
+      <c r="J39" t="s">
+        <v>32</v>
+      </c>
+      <c r="K39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="C40" s="5" t="b">
+        <f>C37&gt;C95</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="5" t="b">
+        <f t="shared" ref="D40:L40" si="21">D37&gt;D95</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="5" t="b">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="5" t="b">
+        <f>IF(COUNTIF(C40:L40, "TRUE") = 0, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B48" t="s">
         <v>5</v>
-      </c>
-      <c r="C37" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>16</v>
       </c>
       <c r="C48" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C49" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C50" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C51" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C52" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C53" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C54" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C55" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C56" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" t="s">
-        <v>34</v>
-      </c>
-      <c r="D58" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" t="s">
-        <v>29</v>
-      </c>
-      <c r="H58" t="s">
-        <v>27</v>
-      </c>
-      <c r="I58" t="s">
-        <v>31</v>
-      </c>
-      <c r="J58" t="s">
-        <v>32</v>
-      </c>
-      <c r="K58" t="s">
-        <v>26</v>
-      </c>
-      <c r="L58" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C59" s="4">
-        <v>6.1</v>
-      </c>
-      <c r="D59" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E59" s="4">
-        <v>10.1</v>
-      </c>
-      <c r="F59" s="4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G59" s="4">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H59" s="4">
-        <v>8.1</v>
-      </c>
-      <c r="I59" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="J59" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="K59" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="L59" s="4">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="4">
         <v>6</v>
       </c>
-      <c r="C60" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="D60" s="4">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="E60" s="4">
-        <v>6.2</v>
-      </c>
-      <c r="F60" s="4">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="G60" s="4">
-        <v>5.2</v>
-      </c>
-      <c r="H60" s="4">
-        <v>7.2</v>
-      </c>
-      <c r="I60" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="J60" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="K60" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L60" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C61" s="4">
-        <v>10.3</v>
-      </c>
-      <c r="D61" s="4">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E61" s="4">
-        <v>6.3</v>
-      </c>
-      <c r="F61" s="4">
-        <v>4.3</v>
-      </c>
-      <c r="G61" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="H61" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I61" s="4">
-        <v>7.3</v>
-      </c>
-      <c r="J61" s="4">
-        <v>3.3</v>
-      </c>
-      <c r="K61" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L61" s="4">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C62" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D62" s="4">
-        <v>9.4</v>
-      </c>
-      <c r="E62" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="F62" s="4">
-        <v>7.4</v>
-      </c>
-      <c r="G62" s="4">
-        <v>5.4</v>
-      </c>
-      <c r="H62" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="I62" s="4">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J62" s="4">
-        <v>8.4</v>
-      </c>
-      <c r="K62" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="L62" s="4">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C63" s="4">
-        <v>4.5</v>
-      </c>
-      <c r="D63" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="E63" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="F63" s="4">
-        <v>10.5</v>
-      </c>
-      <c r="G63" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="H63" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="I63" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="J63" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="K63" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="L63" s="4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C64" s="4">
-        <v>10.6</v>
-      </c>
-      <c r="D64" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="E64" s="4">
-        <v>6.6</v>
-      </c>
-      <c r="F64" s="4">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G64" s="4">
-        <v>8.6</v>
-      </c>
-      <c r="H64" s="4">
-        <v>3.6</v>
-      </c>
-      <c r="I64" s="4">
-        <v>7.6</v>
-      </c>
-      <c r="J64" s="4">
-        <v>5.6</v>
-      </c>
-      <c r="K64" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="L64" s="4">
-        <v>9.6</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C65" s="4">
-        <v>10.7</v>
-      </c>
-      <c r="D65" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="E65" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="F65" s="4">
-        <v>4.7</v>
-      </c>
-      <c r="G65" s="4">
-        <v>5.7</v>
-      </c>
-      <c r="H65" s="4">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="I65" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="J65" s="4">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="K65" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="L65" s="4">
-        <v>7.7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C66" s="4">
-        <v>10.8</v>
-      </c>
-      <c r="D66" s="4">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="E66" s="4">
-        <v>6.8</v>
-      </c>
-      <c r="F66" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="G66" s="4">
-        <v>5.8</v>
-      </c>
-      <c r="H66" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="I66" s="4">
-        <v>7.8</v>
-      </c>
-      <c r="J66" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="K66" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="L66" s="4">
-        <v>8.8000000000000007</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C67" s="4">
-        <v>10.9</v>
-      </c>
-      <c r="D67" s="4">
-        <v>9.9</v>
-      </c>
-      <c r="E67" s="4">
-        <v>6.9</v>
-      </c>
-      <c r="F67" s="4">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G67" s="4">
-        <v>5.9</v>
-      </c>
-      <c r="H67" s="4">
-        <v>3.9</v>
-      </c>
-      <c r="I67" s="4">
-        <v>2.9</v>
-      </c>
-      <c r="J67" s="4">
-        <v>8.9</v>
-      </c>
-      <c r="K67" s="4">
-        <v>7.9</v>
-      </c>
-      <c r="L67" s="4">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" s="4">
-        <v>10.4</v>
-      </c>
-      <c r="D68" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="E68" s="4">
-        <v>6.4</v>
-      </c>
-      <c r="F68" s="4">
-        <v>4.3</v>
-      </c>
-      <c r="G68" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="H68" s="4">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="I68" s="4">
-        <v>6.9</v>
-      </c>
-      <c r="J68" s="4">
-        <v>8.4</v>
-      </c>
-      <c r="K68" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="L68" s="4">
-        <v>5.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="4">
+      <c r="A69" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" t="s">
+        <v>28</v>
+      </c>
+      <c r="G69" t="s">
+        <v>29</v>
+      </c>
+      <c r="H69" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" t="s">
+        <v>31</v>
+      </c>
+      <c r="J69" t="s">
+        <v>32</v>
+      </c>
+      <c r="K69" t="s">
+        <v>26</v>
+      </c>
+      <c r="L69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="D70" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E70" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="F70" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G70" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H70" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="I70" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="J70" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="K70" s="4">
         <v>2.1</v>
       </c>
-      <c r="D69" s="4">
+      <c r="L70" s="4">
         <v>9.1</v>
-      </c>
-      <c r="E69" s="4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F69" s="4">
-        <v>6.1</v>
-      </c>
-      <c r="G69" s="4">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H69" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="I69" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="J69" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K69" s="4">
-        <v>10.1</v>
-      </c>
-      <c r="L69" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="4">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D70" s="4">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="E70" s="4">
-        <v>6.2</v>
-      </c>
-      <c r="F70" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="G70" s="4">
-        <v>5.2</v>
-      </c>
-      <c r="H70" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="I70" s="4">
-        <v>7.2</v>
-      </c>
-      <c r="J70" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="K70" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="L70" s="4">
-        <v>2.1</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C71" s="4">
-        <v>7.3</v>
+        <v>4.2</v>
       </c>
       <c r="D71" s="4">
-        <v>3.3</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E71" s="4">
-        <v>1.3</v>
+        <v>6.2</v>
       </c>
       <c r="F71" s="4">
-        <v>4.3</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="G71" s="4">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="H71" s="4">
-        <v>9.3000000000000007</v>
+        <v>7.2</v>
       </c>
       <c r="I71" s="4">
-        <v>10.3</v>
+        <v>3.2</v>
       </c>
       <c r="J71" s="4">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K71" s="4">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L71" s="4">
-        <v>6.3</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C72" s="4">
-        <v>3.4</v>
+        <v>10.3</v>
       </c>
       <c r="D72" s="4">
-        <v>4.4000000000000004</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E72" s="4">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="F72" s="4">
-        <v>9.4</v>
+        <v>4.3</v>
       </c>
       <c r="G72" s="4">
-        <v>5.4</v>
+        <v>1.3</v>
       </c>
       <c r="H72" s="4">
-        <v>10.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I72" s="4">
-        <v>2.4</v>
+        <v>7.3</v>
       </c>
       <c r="J72" s="4">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="K72" s="4">
-        <v>7.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L72" s="4">
-        <v>8.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C73" s="4">
-        <v>5.5</v>
+        <v>2.4</v>
       </c>
       <c r="D73" s="4">
-        <v>1.5</v>
+        <v>9.4</v>
       </c>
       <c r="E73" s="4">
-        <v>6.5</v>
+        <v>1.4</v>
       </c>
       <c r="F73" s="4">
-        <v>4.5</v>
+        <v>7.4</v>
       </c>
       <c r="G73" s="4">
-        <v>10.5</v>
+        <v>5.4</v>
       </c>
       <c r="H73" s="4">
-        <v>8.5</v>
+        <v>3.4</v>
       </c>
       <c r="I73" s="4">
-        <v>7.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J73" s="4">
-        <v>3.5</v>
+        <v>8.4</v>
       </c>
       <c r="K73" s="4">
-        <v>2.5</v>
+        <v>10.4</v>
       </c>
       <c r="L73" s="4">
-        <v>9.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C74" s="4">
-        <v>10.6</v>
+        <v>4.5</v>
       </c>
       <c r="D74" s="4">
-        <v>4.5999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="E74" s="4">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="F74" s="4">
-        <v>5.6</v>
+        <v>10.5</v>
       </c>
       <c r="G74" s="4">
-        <v>9.6</v>
+        <v>9.5</v>
       </c>
       <c r="H74" s="4">
-        <v>8.6</v>
+        <v>1.5</v>
       </c>
       <c r="I74" s="4">
-        <v>1.6</v>
+        <v>7.5</v>
       </c>
       <c r="J74" s="4">
-        <v>3.6</v>
+        <v>8.5</v>
       </c>
       <c r="K74" s="4">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="L74" s="4">
-        <v>7.6</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C75" s="4">
-        <v>3.7</v>
+        <v>10.6</v>
       </c>
       <c r="D75" s="4">
-        <v>5.7</v>
+        <v>1.6</v>
       </c>
       <c r="E75" s="4">
-        <v>10.7</v>
+        <v>6.6</v>
       </c>
       <c r="F75" s="4">
-        <v>1.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G75" s="4">
-        <v>9.6999999999999993</v>
+        <v>8.6</v>
       </c>
       <c r="H75" s="4">
-        <v>6.7</v>
+        <v>3.6</v>
       </c>
       <c r="I75" s="4">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
       <c r="J75" s="4">
-        <v>8.6999999999999993</v>
+        <v>5.6</v>
       </c>
       <c r="K75" s="4">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="L75" s="4">
-        <v>4.7</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C76" s="4">
-        <v>10.8</v>
+        <v>10.7</v>
       </c>
       <c r="D76" s="4">
-        <v>1.8</v>
+        <v>3.7</v>
       </c>
       <c r="E76" s="4">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="F76" s="4">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="G76" s="4">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="H76" s="4">
-        <v>3.8</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="I76" s="4">
-        <v>7.8</v>
+        <v>1.7</v>
       </c>
       <c r="J76" s="4">
-        <v>8.8000000000000007</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="K76" s="4">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="L76" s="4">
-        <v>9.8000000000000007</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C77" s="4">
-        <v>1.9</v>
+        <v>10.8</v>
       </c>
       <c r="D77" s="4">
-        <v>9.9</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E77" s="4">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="F77" s="4">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="G77" s="4">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="H77" s="4">
-        <v>7.9</v>
+        <v>1.8</v>
       </c>
       <c r="I77" s="4">
-        <v>3.9</v>
+        <v>7.8</v>
       </c>
       <c r="J77" s="4">
-        <v>8.9</v>
+        <v>1.8</v>
       </c>
       <c r="K77" s="4">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="L77" s="4">
-        <v>10.9</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="4">
+        <v>10.9</v>
+      </c>
+      <c r="D78" s="4">
+        <v>9.9</v>
+      </c>
+      <c r="E78" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="F78" s="4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G78" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="H78" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="I78" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="J78" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="K78" s="4">
+        <v>7.9</v>
+      </c>
+      <c r="L78" s="4">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="4">
+        <v>10.4</v>
+      </c>
+      <c r="D79" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="E79" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="F79" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="G79" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="H79" s="4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I79" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="J79" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="K79" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="L79" s="4">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D80" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="E80" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F80" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="G80" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H80" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="I80" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="J80" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K80" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="L80" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D81" s="4">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E81" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="F81" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G81" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="H81" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="I81" s="4">
+        <v>7.2</v>
+      </c>
+      <c r="J81" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="K81" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="L81" s="4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="4">
+        <v>7.3</v>
+      </c>
+      <c r="D82" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="E82" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="F82" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="G82" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="H82" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I82" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="J82" s="4">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K82" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L82" s="4">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="D83" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E83" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="F83" s="4">
+        <v>9.4</v>
+      </c>
+      <c r="G83" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="H83" s="4">
+        <v>10.4</v>
+      </c>
+      <c r="I83" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="J83" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="K83" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="L83" s="4">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="D84" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E84" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="F84" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="G84" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="H84" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="I84" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="J84" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="K84" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L84" s="4">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="D85" s="4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E85" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="F85" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="G85" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="H85" s="4">
+        <v>8.6</v>
+      </c>
+      <c r="I85" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J85" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="K85" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="L85" s="4">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="D86" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="E86" s="4">
+        <v>10.7</v>
+      </c>
+      <c r="F86" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="G86" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H86" s="4">
+        <v>6.7</v>
+      </c>
+      <c r="I86" s="4">
+        <v>7.7</v>
+      </c>
+      <c r="J86" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K86" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="L86" s="4">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="4">
+        <v>10.8</v>
+      </c>
+      <c r="D87" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="E87" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="F87" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="G87" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="H87" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="I87" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="J87" s="4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K87" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="L87" s="4">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="D88" s="4">
+        <v>9.9</v>
+      </c>
+      <c r="E88" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="F88" s="4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G88" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="H88" s="4">
+        <v>7.9</v>
+      </c>
+      <c r="I88" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="J88" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="K88" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="L88" s="4">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
         <v>24</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C89" s="4">
         <v>2.9</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D89" s="4">
         <v>5.4</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E89" s="4">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F78" s="4">
+      <c r="F89" s="4">
         <v>5.5</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G89" s="4">
         <v>4.7</v>
       </c>
-      <c r="H78" s="4">
+      <c r="H89" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I78" s="4">
+      <c r="I89" s="4">
         <v>6.4</v>
       </c>
-      <c r="J78" s="4">
+      <c r="J89" s="4">
         <v>7.8</v>
       </c>
-      <c r="K78" s="4">
+      <c r="K89" s="4">
         <v>3.4</v>
       </c>
-      <c r="L78" s="4">
+      <c r="L89" s="4">
         <v>4.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C80" t="s">
-        <v>34</v>
-      </c>
-      <c r="D80" t="s">
-        <v>33</v>
-      </c>
-      <c r="E80" t="s">
-        <v>30</v>
-      </c>
-      <c r="F80" t="s">
-        <v>28</v>
-      </c>
-      <c r="G80" t="s">
-        <v>29</v>
-      </c>
-      <c r="H80" t="s">
-        <v>27</v>
-      </c>
-      <c r="I80" t="s">
-        <v>31</v>
-      </c>
-      <c r="J80" t="s">
-        <v>32</v>
-      </c>
-      <c r="K80" t="s">
-        <v>26</v>
-      </c>
-      <c r="L80" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>2</v>
-      </c>
-      <c r="C81" s="4">
-        <v>55</v>
-      </c>
-      <c r="D81" s="4">
-        <v>45</v>
-      </c>
-      <c r="E81" s="4">
-        <v>40</v>
-      </c>
-      <c r="F81" s="4">
-        <v>45</v>
-      </c>
-      <c r="G81" s="4">
-        <v>50</v>
-      </c>
-      <c r="H81" s="4">
-        <v>45</v>
-      </c>
-      <c r="I81" s="4">
-        <v>35</v>
-      </c>
-      <c r="J81" s="4">
-        <v>40</v>
-      </c>
-      <c r="K81" s="4">
-        <v>50</v>
-      </c>
-      <c r="L81" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C83" t="s">
-        <v>34</v>
-      </c>
-      <c r="D83" t="s">
-        <v>33</v>
-      </c>
-      <c r="E83" t="s">
-        <v>30</v>
-      </c>
-      <c r="F83" t="s">
-        <v>28</v>
-      </c>
-      <c r="G83" t="s">
-        <v>29</v>
-      </c>
-      <c r="H83" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" t="s">
-        <v>31</v>
-      </c>
-      <c r="J83" t="s">
-        <v>32</v>
-      </c>
-      <c r="K83" t="s">
-        <v>26</v>
-      </c>
-      <c r="L83" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="4">
-        <v>35</v>
-      </c>
-      <c r="D84" s="4">
-        <v>60</v>
-      </c>
-      <c r="E84" s="4">
-        <v>48</v>
-      </c>
-      <c r="F84" s="4">
-        <v>55</v>
-      </c>
-      <c r="G84" s="4">
-        <v>45</v>
-      </c>
-      <c r="H84" s="4">
-        <v>50</v>
-      </c>
-      <c r="I84" s="4">
-        <v>36</v>
-      </c>
-      <c r="J84" s="4">
-        <v>50</v>
-      </c>
-      <c r="K84" s="4">
-        <v>40</v>
-      </c>
-      <c r="L84" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="7"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="7"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C88" t="s">
-        <v>34</v>
-      </c>
-      <c r="D88" t="s">
-        <v>33</v>
-      </c>
-      <c r="E88" t="s">
-        <v>30</v>
-      </c>
-      <c r="F88" t="s">
-        <v>28</v>
-      </c>
-      <c r="G88" t="s">
-        <v>29</v>
-      </c>
-      <c r="H88" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" t="s">
-        <v>31</v>
-      </c>
-      <c r="J88" t="s">
-        <v>32</v>
-      </c>
-      <c r="K88" t="s">
-        <v>26</v>
-      </c>
-      <c r="L88" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="C89" s="5">
-        <f>C81*C8</f>
-        <v>55</v>
-      </c>
-      <c r="D89" s="5">
-        <f t="shared" ref="D89:L89" si="20">D81*D8</f>
-        <v>45</v>
-      </c>
-      <c r="E89" s="5">
-        <f t="shared" si="20"/>
-        <v>40</v>
-      </c>
-      <c r="F89" s="5">
-        <f t="shared" si="20"/>
-        <v>45</v>
-      </c>
-      <c r="G89" s="5">
-        <f t="shared" si="20"/>
-        <v>50</v>
-      </c>
-      <c r="H89" s="5">
-        <f t="shared" si="20"/>
-        <v>45</v>
-      </c>
-      <c r="I89" s="5">
-        <f t="shared" si="20"/>
-        <v>35</v>
-      </c>
-      <c r="J89" s="5">
-        <f t="shared" si="20"/>
-        <v>40</v>
-      </c>
-      <c r="K89" s="5">
-        <f t="shared" si="20"/>
-        <v>50</v>
-      </c>
-      <c r="L89" s="5">
-        <f t="shared" si="20"/>
-        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C91" t="s">
         <v>34</v>
@@ -2838,917 +2793,1150 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="4">
+        <v>55</v>
+      </c>
+      <c r="D92" s="4">
+        <v>45</v>
+      </c>
+      <c r="E92" s="4">
+        <v>40</v>
+      </c>
+      <c r="F92" s="4">
+        <v>45</v>
+      </c>
+      <c r="G92" s="4">
+        <v>50</v>
+      </c>
+      <c r="H92" s="4">
+        <v>45</v>
+      </c>
+      <c r="I92" s="4">
+        <v>35</v>
+      </c>
+      <c r="J92" s="4">
+        <v>40</v>
+      </c>
+      <c r="K92" s="4">
+        <v>50</v>
+      </c>
+      <c r="L92" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" t="s">
+        <v>34</v>
+      </c>
+      <c r="D94" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" t="s">
+        <v>28</v>
+      </c>
+      <c r="G94" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" t="s">
+        <v>31</v>
+      </c>
+      <c r="J94" t="s">
+        <v>32</v>
+      </c>
+      <c r="K94" t="s">
+        <v>26</v>
+      </c>
+      <c r="L94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="4">
+        <v>35</v>
+      </c>
+      <c r="D95" s="4">
+        <v>60</v>
+      </c>
+      <c r="E95" s="4">
+        <v>48</v>
+      </c>
+      <c r="F95" s="4">
+        <v>55</v>
+      </c>
+      <c r="G95" s="4">
+        <v>45</v>
+      </c>
+      <c r="H95" s="4">
+        <v>50</v>
+      </c>
+      <c r="I95" s="4">
+        <v>36</v>
+      </c>
+      <c r="J95" s="4">
+        <v>50</v>
+      </c>
+      <c r="K95" s="4">
+        <v>40</v>
+      </c>
+      <c r="L95" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" t="s">
+        <v>34</v>
+      </c>
+      <c r="D99" t="s">
+        <v>33</v>
+      </c>
+      <c r="E99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F99" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" t="s">
+        <v>27</v>
+      </c>
+      <c r="I99" t="s">
+        <v>31</v>
+      </c>
+      <c r="J99" t="s">
+        <v>32</v>
+      </c>
+      <c r="K99" t="s">
+        <v>26</v>
+      </c>
+      <c r="L99" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="C100" s="5">
+        <f>C92*C8</f>
+        <v>55</v>
+      </c>
+      <c r="D100" s="5">
+        <f t="shared" ref="D100:L100" si="22">D92*D8</f>
+        <v>45</v>
+      </c>
+      <c r="E100" s="5">
+        <f t="shared" si="22"/>
+        <v>40</v>
+      </c>
+      <c r="F100" s="5">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="G100" s="5">
+        <f t="shared" si="22"/>
+        <v>50</v>
+      </c>
+      <c r="H100" s="5">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="I100" s="5">
+        <f t="shared" si="22"/>
+        <v>35</v>
+      </c>
+      <c r="J100" s="5">
+        <f t="shared" si="22"/>
+        <v>40</v>
+      </c>
+      <c r="K100" s="5">
+        <f t="shared" si="22"/>
+        <v>50</v>
+      </c>
+      <c r="L100" s="5">
+        <f t="shared" si="22"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" t="s">
+        <v>34</v>
+      </c>
+      <c r="D102" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" t="s">
+        <v>30</v>
+      </c>
+      <c r="F102" t="s">
+        <v>28</v>
+      </c>
+      <c r="G102" t="s">
+        <v>29</v>
+      </c>
+      <c r="H102" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" t="s">
+        <v>31</v>
+      </c>
+      <c r="J102" t="s">
+        <v>32</v>
+      </c>
+      <c r="K102" t="s">
+        <v>26</v>
+      </c>
+      <c r="L102" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="5">
-        <f>C59*C13</f>
+      <c r="C103" s="5">
+        <f>C70*C13</f>
         <v>3.6599999999999997</v>
       </c>
-      <c r="D92" s="5">
-        <f t="shared" ref="D92:L92" si="21">D59*D13</f>
+      <c r="D103" s="5">
+        <f t="shared" ref="D103:L103" si="23">D70*D13</f>
         <v>0.66</v>
       </c>
-      <c r="E92" s="5">
-        <f t="shared" si="21"/>
+      <c r="E103" s="5">
+        <f t="shared" si="23"/>
         <v>6.06</v>
       </c>
-      <c r="F92" s="5">
-        <f t="shared" si="21"/>
+      <c r="F103" s="5">
+        <f t="shared" si="23"/>
         <v>2.4599999999999995</v>
       </c>
-      <c r="G92" s="5">
-        <f t="shared" si="21"/>
+      <c r="G103" s="5">
+        <f t="shared" si="23"/>
         <v>3.0599999999999996</v>
       </c>
-      <c r="H92" s="5">
-        <f t="shared" si="21"/>
+      <c r="H103" s="5">
+        <f t="shared" si="23"/>
         <v>4.8599999999999994</v>
       </c>
-      <c r="I92" s="5">
-        <f t="shared" si="21"/>
+      <c r="I103" s="5">
+        <f t="shared" si="23"/>
         <v>4.26</v>
       </c>
-      <c r="J92" s="5">
-        <f t="shared" si="21"/>
+      <c r="J103" s="5">
+        <f t="shared" si="23"/>
         <v>1.8599999999999999</v>
       </c>
-      <c r="K92" s="5">
-        <f t="shared" si="21"/>
+      <c r="K103" s="5">
+        <f t="shared" si="23"/>
         <v>1.26</v>
       </c>
-      <c r="L92" s="5">
-        <f t="shared" si="21"/>
+      <c r="L103" s="5">
+        <f t="shared" si="23"/>
         <v>5.46</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="104" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="5">
-        <f t="shared" ref="C93:L93" si="22">C60*C14</f>
+      <c r="C104" s="5">
+        <f t="shared" ref="C104:L104" si="24">C71*C14</f>
         <v>2.52</v>
       </c>
-      <c r="D93" s="5">
-        <f t="shared" si="22"/>
+      <c r="D104" s="5">
+        <f t="shared" si="24"/>
         <v>5.52</v>
       </c>
-      <c r="E93" s="5">
-        <f t="shared" si="22"/>
+      <c r="E104" s="5">
+        <f t="shared" si="24"/>
         <v>3.7199999999999998</v>
       </c>
-      <c r="F93" s="5">
-        <f t="shared" si="22"/>
+      <c r="F104" s="5">
+        <f t="shared" si="24"/>
         <v>6.1199999999999992</v>
       </c>
-      <c r="G93" s="5">
-        <f t="shared" si="22"/>
+      <c r="G104" s="5">
+        <f t="shared" si="24"/>
         <v>3.12</v>
       </c>
-      <c r="H93" s="5">
-        <f t="shared" si="22"/>
+      <c r="H104" s="5">
+        <f t="shared" si="24"/>
         <v>4.32</v>
       </c>
-      <c r="I93" s="5">
-        <f t="shared" si="22"/>
+      <c r="I104" s="5">
+        <f t="shared" si="24"/>
         <v>1.92</v>
       </c>
-      <c r="J93" s="5">
-        <f t="shared" si="22"/>
+      <c r="J104" s="5">
+        <f t="shared" si="24"/>
         <v>4.919999999999999</v>
       </c>
-      <c r="K93" s="5">
-        <f t="shared" si="22"/>
+      <c r="K104" s="5">
+        <f t="shared" si="24"/>
         <v>1.32</v>
       </c>
-      <c r="L93" s="5">
-        <f t="shared" si="22"/>
+      <c r="L104" s="5">
+        <f t="shared" si="24"/>
         <v>4.919999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
+    <row r="105" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
         <v>7</v>
       </c>
-      <c r="C94" s="5">
-        <f t="shared" ref="C94:L94" si="23">C61*C15</f>
+      <c r="C105" s="5">
+        <f t="shared" ref="C105:L105" si="25">C72*C15</f>
         <v>6.1800000000000006</v>
       </c>
-      <c r="D94" s="5">
-        <f t="shared" si="23"/>
+      <c r="D105" s="5">
+        <f t="shared" si="25"/>
         <v>5.58</v>
       </c>
-      <c r="E94" s="5">
-        <f t="shared" si="23"/>
+      <c r="E105" s="5">
+        <f t="shared" si="25"/>
         <v>3.78</v>
       </c>
-      <c r="F94" s="5">
-        <f t="shared" si="23"/>
+      <c r="F105" s="5">
+        <f t="shared" si="25"/>
         <v>2.5799999999999996</v>
       </c>
-      <c r="G94" s="5">
-        <f t="shared" si="23"/>
+      <c r="G105" s="5">
+        <f t="shared" si="25"/>
         <v>0.78</v>
       </c>
-      <c r="H94" s="5">
-        <f t="shared" si="23"/>
+      <c r="H105" s="5">
+        <f t="shared" si="25"/>
         <v>4.9800000000000004</v>
       </c>
-      <c r="I94" s="5">
-        <f t="shared" si="23"/>
+      <c r="I105" s="5">
+        <f t="shared" si="25"/>
         <v>4.38</v>
       </c>
-      <c r="J94" s="5">
-        <f t="shared" si="23"/>
+      <c r="J105" s="5">
+        <f t="shared" si="25"/>
         <v>1.9799999999999998</v>
       </c>
-      <c r="K94" s="5">
-        <f t="shared" si="23"/>
+      <c r="K105" s="5">
+        <f t="shared" si="25"/>
         <v>1.38</v>
       </c>
-      <c r="L94" s="5">
-        <f t="shared" si="23"/>
+      <c r="L105" s="5">
+        <f t="shared" si="25"/>
         <v>3.1799999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
+    <row r="106" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="5">
-        <f t="shared" ref="C95:L95" si="24">C62*C16</f>
+      <c r="C106" s="5">
+        <f t="shared" ref="C106:L106" si="26">C73*C16</f>
         <v>1.44</v>
       </c>
-      <c r="D95" s="5">
-        <f t="shared" si="24"/>
+      <c r="D106" s="5">
+        <f t="shared" si="26"/>
         <v>5.64</v>
       </c>
-      <c r="E95" s="5">
-        <f t="shared" si="24"/>
+      <c r="E106" s="5">
+        <f t="shared" si="26"/>
         <v>0.84</v>
       </c>
-      <c r="F95" s="5">
-        <f t="shared" si="24"/>
+      <c r="F106" s="5">
+        <f t="shared" si="26"/>
         <v>4.4400000000000004</v>
       </c>
-      <c r="G95" s="5">
-        <f t="shared" si="24"/>
+      <c r="G106" s="5">
+        <f t="shared" si="26"/>
         <v>3.24</v>
       </c>
-      <c r="H95" s="5">
-        <f t="shared" si="24"/>
+      <c r="H106" s="5">
+        <f t="shared" si="26"/>
         <v>2.04</v>
       </c>
-      <c r="I95" s="5">
-        <f t="shared" si="24"/>
+      <c r="I106" s="5">
+        <f t="shared" si="26"/>
         <v>2.64</v>
       </c>
-      <c r="J95" s="5">
-        <f t="shared" si="24"/>
+      <c r="J106" s="5">
+        <f t="shared" si="26"/>
         <v>5.04</v>
       </c>
-      <c r="K95" s="5">
-        <f t="shared" si="24"/>
+      <c r="K106" s="5">
+        <f t="shared" si="26"/>
         <v>6.24</v>
       </c>
-      <c r="L95" s="5">
-        <f t="shared" si="24"/>
+      <c r="L106" s="5">
+        <f t="shared" si="26"/>
         <v>3.84</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
+    <row r="107" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
         <v>9</v>
       </c>
-      <c r="C96" s="5">
-        <f t="shared" ref="C96:L96" si="25">C63*C17</f>
+      <c r="C107" s="5">
+        <f t="shared" ref="C107:L107" si="27">C74*C17</f>
         <v>2.6999999999999997</v>
       </c>
-      <c r="D96" s="5">
-        <f t="shared" si="25"/>
+      <c r="D107" s="5">
+        <f t="shared" si="27"/>
         <v>3.3</v>
       </c>
-      <c r="E96" s="5">
-        <f t="shared" si="25"/>
+      <c r="E107" s="5">
+        <f t="shared" si="27"/>
         <v>3.9</v>
       </c>
-      <c r="F96" s="5">
-        <f t="shared" si="25"/>
+      <c r="F107" s="5">
+        <f t="shared" si="27"/>
         <v>6.3</v>
       </c>
-      <c r="G96" s="5">
-        <f t="shared" si="25"/>
+      <c r="G107" s="5">
+        <f t="shared" si="27"/>
         <v>5.7</v>
       </c>
-      <c r="H96" s="5">
-        <f t="shared" si="25"/>
+      <c r="H107" s="5">
+        <f t="shared" si="27"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="I96" s="5">
-        <f t="shared" si="25"/>
+      <c r="I107" s="5">
+        <f t="shared" si="27"/>
         <v>4.5</v>
       </c>
-      <c r="J96" s="5">
-        <f t="shared" si="25"/>
+      <c r="J107" s="5">
+        <f t="shared" si="27"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="K96" s="5">
-        <f t="shared" si="25"/>
+      <c r="K107" s="5">
+        <f t="shared" si="27"/>
         <v>1.5</v>
       </c>
-      <c r="L96" s="5">
-        <f t="shared" si="25"/>
+      <c r="L107" s="5">
+        <f t="shared" si="27"/>
         <v>2.1</v>
       </c>
     </row>
-    <row r="97" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
+    <row r="108" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
         <v>10</v>
       </c>
-      <c r="C97" s="5">
-        <f t="shared" ref="C97:L97" si="26">C64*C18</f>
+      <c r="C108" s="5">
+        <f t="shared" ref="C108:L108" si="28">C75*C18</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D97" s="5">
-        <f t="shared" si="26"/>
+      <c r="D108" s="5">
+        <f t="shared" si="28"/>
         <v>0.96</v>
       </c>
-      <c r="E97" s="5">
-        <f t="shared" si="26"/>
+      <c r="E108" s="5">
+        <f t="shared" si="28"/>
         <v>3.9599999999999995</v>
       </c>
-      <c r="F97" s="5">
-        <f t="shared" si="26"/>
+      <c r="F108" s="5">
+        <f t="shared" si="28"/>
         <v>2.76</v>
       </c>
-      <c r="G97" s="5">
-        <f t="shared" si="26"/>
+      <c r="G108" s="5">
+        <f t="shared" si="28"/>
         <v>5.1599999999999993</v>
       </c>
-      <c r="H97" s="5">
-        <f t="shared" si="26"/>
+      <c r="H108" s="5">
+        <f t="shared" si="28"/>
         <v>2.16</v>
       </c>
-      <c r="I97" s="5">
-        <f t="shared" si="26"/>
+      <c r="I108" s="5">
+        <f t="shared" si="28"/>
         <v>4.5599999999999996</v>
       </c>
-      <c r="J97" s="5">
-        <f t="shared" si="26"/>
+      <c r="J108" s="5">
+        <f t="shared" si="28"/>
         <v>3.36</v>
       </c>
-      <c r="K97" s="5">
-        <f t="shared" si="26"/>
+      <c r="K108" s="5">
+        <f t="shared" si="28"/>
         <v>1.56</v>
       </c>
-      <c r="L97" s="5">
-        <f t="shared" si="26"/>
+      <c r="L108" s="5">
+        <f t="shared" si="28"/>
         <v>5.76</v>
       </c>
     </row>
-    <row r="98" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
+    <row r="109" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="5">
-        <f t="shared" ref="C98:L98" si="27">C65*C19</f>
+      <c r="C109" s="5">
+        <f t="shared" ref="C109:L109" si="29">C76*C19</f>
         <v>6.419999999999999</v>
       </c>
-      <c r="D98" s="5">
-        <f t="shared" si="27"/>
+      <c r="D109" s="5">
+        <f t="shared" si="29"/>
         <v>2.2200000000000002</v>
       </c>
-      <c r="E98" s="5">
-        <f t="shared" si="27"/>
+      <c r="E109" s="5">
+        <f t="shared" si="29"/>
         <v>4.0199999999999996</v>
       </c>
-      <c r="F98" s="5">
-        <f t="shared" si="27"/>
+      <c r="F109" s="5">
+        <f t="shared" si="29"/>
         <v>2.82</v>
       </c>
-      <c r="G98" s="5">
-        <f t="shared" si="27"/>
+      <c r="G109" s="5">
+        <f t="shared" si="29"/>
         <v>3.42</v>
       </c>
-      <c r="H98" s="5">
-        <f t="shared" si="27"/>
+      <c r="H109" s="5">
+        <f t="shared" si="29"/>
         <v>5.8199999999999994</v>
       </c>
-      <c r="I98" s="5">
-        <f t="shared" si="27"/>
+      <c r="I109" s="5">
+        <f t="shared" si="29"/>
         <v>1.02</v>
       </c>
-      <c r="J98" s="5">
-        <f t="shared" si="27"/>
+      <c r="J109" s="5">
+        <f t="shared" si="29"/>
         <v>5.22</v>
       </c>
-      <c r="K98" s="5">
-        <f t="shared" si="27"/>
+      <c r="K109" s="5">
+        <f t="shared" si="29"/>
         <v>1.62</v>
       </c>
-      <c r="L98" s="5">
-        <f t="shared" si="27"/>
+      <c r="L109" s="5">
+        <f t="shared" si="29"/>
         <v>4.62</v>
       </c>
     </row>
-    <row r="99" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
+    <row r="110" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
         <v>12</v>
       </c>
-      <c r="C99" s="5">
-        <f t="shared" ref="C99:L99" si="28">C66*C20</f>
+      <c r="C110" s="5">
+        <f t="shared" ref="C110:L110" si="30">C77*C20</f>
         <v>6.48</v>
       </c>
-      <c r="D99" s="5">
-        <f t="shared" si="28"/>
+      <c r="D110" s="5">
+        <f t="shared" si="30"/>
         <v>5.88</v>
       </c>
-      <c r="E99" s="5">
-        <f t="shared" si="28"/>
+      <c r="E110" s="5">
+        <f t="shared" si="30"/>
         <v>4.08</v>
       </c>
-      <c r="F99" s="5">
-        <f t="shared" si="28"/>
+      <c r="F110" s="5">
+        <f t="shared" si="30"/>
         <v>2.88</v>
       </c>
-      <c r="G99" s="5">
-        <f t="shared" si="28"/>
+      <c r="G110" s="5">
+        <f t="shared" si="30"/>
         <v>3.48</v>
       </c>
-      <c r="H99" s="5">
-        <f t="shared" si="28"/>
+      <c r="H110" s="5">
+        <f t="shared" si="30"/>
         <v>1.08</v>
       </c>
-      <c r="I99" s="5">
-        <f t="shared" si="28"/>
+      <c r="I110" s="5">
+        <f t="shared" si="30"/>
         <v>4.68</v>
       </c>
-      <c r="J99" s="5">
-        <f t="shared" si="28"/>
+      <c r="J110" s="5">
+        <f t="shared" si="30"/>
         <v>1.08</v>
       </c>
-      <c r="K99" s="5">
-        <f t="shared" si="28"/>
+      <c r="K110" s="5">
+        <f t="shared" si="30"/>
         <v>1.68</v>
       </c>
-      <c r="L99" s="5">
-        <f t="shared" si="28"/>
-        <v>5.28</v>
-      </c>
-    </row>
-    <row r="100" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B100" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" s="5">
-        <f t="shared" ref="C100:L100" si="29">C67*C21</f>
-        <v>6.54</v>
-      </c>
-      <c r="D100" s="5">
-        <f t="shared" si="29"/>
-        <v>5.94</v>
-      </c>
-      <c r="E100" s="5">
-        <f t="shared" si="29"/>
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="F100" s="5">
-        <f t="shared" si="29"/>
-        <v>2.94</v>
-      </c>
-      <c r="G100" s="5">
-        <f t="shared" si="29"/>
-        <v>3.54</v>
-      </c>
-      <c r="H100" s="5">
-        <f t="shared" si="29"/>
-        <v>2.34</v>
-      </c>
-      <c r="I100" s="5">
-        <f t="shared" si="29"/>
-        <v>1.74</v>
-      </c>
-      <c r="J100" s="5">
-        <f t="shared" si="29"/>
-        <v>5.34</v>
-      </c>
-      <c r="K100" s="5">
-        <f t="shared" si="29"/>
-        <v>4.74</v>
-      </c>
-      <c r="L100" s="5">
-        <f t="shared" si="29"/>
-        <v>2.34</v>
-      </c>
-    </row>
-    <row r="101" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>14</v>
-      </c>
-      <c r="C101" s="5">
-        <f t="shared" ref="C101:L101" si="30">C68*C22</f>
-        <v>6.24</v>
-      </c>
-      <c r="D101" s="5">
-        <f t="shared" si="30"/>
-        <v>1.92</v>
-      </c>
-      <c r="E101" s="5">
-        <f t="shared" si="30"/>
-        <v>3.84</v>
-      </c>
-      <c r="F101" s="5">
-        <f t="shared" si="30"/>
-        <v>2.5799999999999996</v>
-      </c>
-      <c r="G101" s="5">
-        <f t="shared" si="30"/>
-        <v>0.78</v>
-      </c>
-      <c r="H101" s="5">
+      <c r="L110" s="5">
         <f t="shared" si="30"/>
         <v>5.28</v>
       </c>
-      <c r="I101" s="5">
-        <f t="shared" si="30"/>
+    </row>
+    <row r="111" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111" s="5">
+        <f t="shared" ref="C111:L111" si="31">C78*C21</f>
+        <v>6.54</v>
+      </c>
+      <c r="D111" s="5">
+        <f t="shared" si="31"/>
+        <v>5.94</v>
+      </c>
+      <c r="E111" s="5">
+        <f t="shared" si="31"/>
         <v>4.1399999999999997</v>
       </c>
-      <c r="J101" s="5">
-        <f t="shared" si="30"/>
-        <v>5.04</v>
-      </c>
-      <c r="K101" s="5">
-        <f t="shared" si="30"/>
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="L101" s="5">
-        <f t="shared" si="30"/>
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="102" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
-        <v>15</v>
-      </c>
-      <c r="C102" s="5">
-        <f t="shared" ref="C102:L102" si="31">C69*C23</f>
-        <v>1.26</v>
-      </c>
-      <c r="D102" s="5">
+      <c r="F111" s="5">
         <f t="shared" si="31"/>
-        <v>5.46</v>
-      </c>
-      <c r="E102" s="5">
+        <v>2.94</v>
+      </c>
+      <c r="G111" s="5">
         <f t="shared" si="31"/>
-        <v>2.4599999999999995</v>
-      </c>
-      <c r="F102" s="5">
+        <v>3.54</v>
+      </c>
+      <c r="H111" s="5">
         <f t="shared" si="31"/>
-        <v>3.6599999999999997</v>
-      </c>
-      <c r="G102" s="5">
+        <v>2.34</v>
+      </c>
+      <c r="I111" s="5">
         <f t="shared" si="31"/>
-        <v>3.0599999999999996</v>
-      </c>
-      <c r="H102" s="5">
+        <v>1.74</v>
+      </c>
+      <c r="J111" s="5">
         <f t="shared" si="31"/>
-        <v>1.8599999999999999</v>
-      </c>
-      <c r="I102" s="5">
+        <v>5.34</v>
+      </c>
+      <c r="K111" s="5">
         <f t="shared" si="31"/>
-        <v>4.26</v>
-      </c>
-      <c r="J102" s="5">
+        <v>4.74</v>
+      </c>
+      <c r="L111" s="5">
         <f t="shared" si="31"/>
-        <v>0.66</v>
-      </c>
-      <c r="K102" s="5">
-        <f t="shared" si="31"/>
-        <v>6.06</v>
-      </c>
-      <c r="L102" s="5">
-        <f t="shared" si="31"/>
-        <v>4.919999999999999</v>
-      </c>
-    </row>
-    <row r="103" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B103" t="s">
-        <v>16</v>
-      </c>
-      <c r="C103" s="5">
-        <f t="shared" ref="C103:L103" si="32">C70*C24</f>
-        <v>6.1199999999999992</v>
-      </c>
-      <c r="D103" s="5">
-        <f t="shared" si="32"/>
-        <v>5.52</v>
-      </c>
-      <c r="E103" s="5">
-        <f t="shared" si="32"/>
-        <v>3.7199999999999998</v>
-      </c>
-      <c r="F103" s="5">
-        <f t="shared" si="32"/>
-        <v>4.919999999999999</v>
-      </c>
-      <c r="G103" s="5">
-        <f t="shared" si="32"/>
-        <v>3.12</v>
-      </c>
-      <c r="H103" s="5">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" s="5">
+        <f t="shared" ref="C112:L112" si="32">C79*C22</f>
+        <v>6.24</v>
+      </c>
+      <c r="D112" s="5">
         <f t="shared" si="32"/>
         <v>1.92</v>
       </c>
-      <c r="I103" s="5">
+      <c r="E112" s="5">
         <f t="shared" si="32"/>
+        <v>3.84</v>
+      </c>
+      <c r="F112" s="5">
+        <f t="shared" si="32"/>
+        <v>2.5799999999999996</v>
+      </c>
+      <c r="G112" s="5">
+        <f t="shared" si="32"/>
+        <v>0.78</v>
+      </c>
+      <c r="H112" s="5">
+        <f t="shared" si="32"/>
+        <v>5.28</v>
+      </c>
+      <c r="I112" s="5">
+        <f t="shared" si="32"/>
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="J112" s="5">
+        <f t="shared" si="32"/>
+        <v>5.04</v>
+      </c>
+      <c r="K112" s="5">
+        <f t="shared" si="32"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="L112" s="5">
+        <f t="shared" si="32"/>
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="5">
+        <f t="shared" ref="C113:L113" si="33">C80*C23</f>
+        <v>1.26</v>
+      </c>
+      <c r="D113" s="5">
+        <f t="shared" si="33"/>
+        <v>5.46</v>
+      </c>
+      <c r="E113" s="5">
+        <f t="shared" si="33"/>
+        <v>2.4599999999999995</v>
+      </c>
+      <c r="F113" s="5">
+        <f t="shared" si="33"/>
+        <v>3.6599999999999997</v>
+      </c>
+      <c r="G113" s="5">
+        <f t="shared" si="33"/>
+        <v>3.0599999999999996</v>
+      </c>
+      <c r="H113" s="5">
+        <f t="shared" si="33"/>
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="I113" s="5">
+        <f t="shared" si="33"/>
+        <v>4.26</v>
+      </c>
+      <c r="J113" s="5">
+        <f t="shared" si="33"/>
+        <v>0.66</v>
+      </c>
+      <c r="K113" s="5">
+        <f t="shared" si="33"/>
+        <v>6.06</v>
+      </c>
+      <c r="L113" s="5">
+        <f t="shared" si="33"/>
+        <v>4.919999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114" s="5">
+        <f t="shared" ref="C114:L114" si="34">C81*C24</f>
+        <v>6.1199999999999992</v>
+      </c>
+      <c r="D114" s="5">
+        <f t="shared" si="34"/>
+        <v>5.52</v>
+      </c>
+      <c r="E114" s="5">
+        <f t="shared" si="34"/>
+        <v>3.7199999999999998</v>
+      </c>
+      <c r="F114" s="5">
+        <f t="shared" si="34"/>
+        <v>4.919999999999999</v>
+      </c>
+      <c r="G114" s="5">
+        <f t="shared" si="34"/>
+        <v>3.12</v>
+      </c>
+      <c r="H114" s="5">
+        <f t="shared" si="34"/>
+        <v>1.92</v>
+      </c>
+      <c r="I114" s="5">
+        <f t="shared" si="34"/>
         <v>4.32</v>
       </c>
-      <c r="J103" s="5">
-        <f t="shared" si="32"/>
+      <c r="J114" s="5">
+        <f t="shared" si="34"/>
         <v>2.52</v>
       </c>
-      <c r="K103" s="5">
-        <f t="shared" si="32"/>
+      <c r="K114" s="5">
+        <f t="shared" si="34"/>
         <v>0.72</v>
       </c>
-      <c r="L103" s="5">
-        <f t="shared" si="32"/>
+      <c r="L114" s="5">
+        <f t="shared" si="34"/>
         <v>1.26</v>
       </c>
     </row>
-    <row r="104" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B104" t="s">
+    <row r="115" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="5">
-        <f t="shared" ref="C104:L104" si="33">C71*C25</f>
+      <c r="C115" s="5">
+        <f t="shared" ref="C115:L115" si="35">C82*C25</f>
         <v>4.38</v>
       </c>
-      <c r="D104" s="5">
-        <f t="shared" si="33"/>
+      <c r="D115" s="5">
+        <f t="shared" si="35"/>
         <v>1.9799999999999998</v>
       </c>
-      <c r="E104" s="5">
-        <f t="shared" si="33"/>
+      <c r="E115" s="5">
+        <f t="shared" si="35"/>
         <v>0.78</v>
       </c>
-      <c r="F104" s="5">
-        <f t="shared" si="33"/>
+      <c r="F115" s="5">
+        <f t="shared" si="35"/>
         <v>2.5799999999999996</v>
       </c>
-      <c r="G104" s="5">
-        <f t="shared" si="33"/>
+      <c r="G115" s="5">
+        <f t="shared" si="35"/>
         <v>3.1799999999999997</v>
       </c>
-      <c r="H104" s="5">
-        <f t="shared" si="33"/>
+      <c r="H115" s="5">
+        <f t="shared" si="35"/>
         <v>5.58</v>
       </c>
-      <c r="I104" s="5">
-        <f t="shared" si="33"/>
+      <c r="I115" s="5">
+        <f t="shared" si="35"/>
         <v>6.1800000000000006</v>
       </c>
-      <c r="J104" s="5">
-        <f t="shared" si="33"/>
+      <c r="J115" s="5">
+        <f t="shared" si="35"/>
         <v>4.9800000000000004</v>
       </c>
-      <c r="K104" s="5">
-        <f t="shared" si="33"/>
+      <c r="K115" s="5">
+        <f t="shared" si="35"/>
         <v>1.38</v>
       </c>
-      <c r="L104" s="5">
-        <f t="shared" si="33"/>
+      <c r="L115" s="5">
+        <f t="shared" si="35"/>
         <v>3.78</v>
       </c>
     </row>
-    <row r="105" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B105" t="s">
+    <row r="116" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
         <v>18</v>
       </c>
-      <c r="C105" s="5">
-        <f t="shared" ref="C105:L105" si="34">C72*C26</f>
+      <c r="C116" s="5">
+        <f t="shared" ref="C116:L116" si="36">C83*C26</f>
         <v>2.04</v>
       </c>
-      <c r="D105" s="5">
-        <f t="shared" si="34"/>
+      <c r="D116" s="5">
+        <f t="shared" si="36"/>
         <v>2.64</v>
       </c>
-      <c r="E105" s="5">
-        <f t="shared" si="34"/>
+      <c r="E116" s="5">
+        <f t="shared" si="36"/>
         <v>3.84</v>
       </c>
-      <c r="F105" s="5">
-        <f t="shared" si="34"/>
+      <c r="F116" s="5">
+        <f t="shared" si="36"/>
         <v>5.64</v>
       </c>
-      <c r="G105" s="5">
-        <f t="shared" si="34"/>
+      <c r="G116" s="5">
+        <f t="shared" si="36"/>
         <v>3.24</v>
       </c>
-      <c r="H105" s="5">
-        <f t="shared" si="34"/>
+      <c r="H116" s="5">
+        <f t="shared" si="36"/>
         <v>6.24</v>
       </c>
-      <c r="I105" s="5">
-        <f t="shared" si="34"/>
+      <c r="I116" s="5">
+        <f t="shared" si="36"/>
         <v>1.44</v>
       </c>
-      <c r="J105" s="5">
-        <f t="shared" si="34"/>
+      <c r="J116" s="5">
+        <f t="shared" si="36"/>
         <v>0.84</v>
       </c>
-      <c r="K105" s="5">
-        <f t="shared" si="34"/>
+      <c r="K116" s="5">
+        <f t="shared" si="36"/>
         <v>4.4400000000000004</v>
       </c>
-      <c r="L105" s="5">
-        <f t="shared" si="34"/>
+      <c r="L116" s="5">
+        <f t="shared" si="36"/>
         <v>5.04</v>
       </c>
     </row>
-    <row r="106" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
+    <row r="117" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
         <v>19</v>
       </c>
-      <c r="C106" s="5">
-        <f t="shared" ref="C106:L106" si="35">C73*C27</f>
+      <c r="C117" s="5">
+        <f t="shared" ref="C117:L117" si="37">C84*C27</f>
         <v>3.3</v>
       </c>
-      <c r="D106" s="5">
-        <f t="shared" si="35"/>
+      <c r="D117" s="5">
+        <f t="shared" si="37"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="E106" s="5">
-        <f t="shared" si="35"/>
+      <c r="E117" s="5">
+        <f t="shared" si="37"/>
         <v>3.9</v>
       </c>
-      <c r="F106" s="5">
-        <f t="shared" si="35"/>
+      <c r="F117" s="5">
+        <f t="shared" si="37"/>
         <v>2.6999999999999997</v>
       </c>
-      <c r="G106" s="5">
-        <f t="shared" si="35"/>
+      <c r="G117" s="5">
+        <f t="shared" si="37"/>
         <v>6.3</v>
       </c>
-      <c r="H106" s="5">
-        <f t="shared" si="35"/>
+      <c r="H117" s="5">
+        <f t="shared" si="37"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="I106" s="5">
-        <f t="shared" si="35"/>
+      <c r="I117" s="5">
+        <f t="shared" si="37"/>
         <v>4.5</v>
       </c>
-      <c r="J106" s="5">
-        <f t="shared" si="35"/>
+      <c r="J117" s="5">
+        <f t="shared" si="37"/>
         <v>2.1</v>
       </c>
-      <c r="K106" s="5">
-        <f t="shared" si="35"/>
+      <c r="K117" s="5">
+        <f t="shared" si="37"/>
         <v>1.5</v>
       </c>
-      <c r="L106" s="5">
-        <f t="shared" si="35"/>
+      <c r="L117" s="5">
+        <f t="shared" si="37"/>
         <v>5.7</v>
       </c>
     </row>
-    <row r="107" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
+    <row r="118" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="5">
-        <f t="shared" ref="C107:L107" si="36">C74*C28</f>
+      <c r="C118" s="5">
+        <f t="shared" ref="C118:L118" si="38">C85*C28</f>
         <v>6.3599999999999994</v>
       </c>
-      <c r="D107" s="5">
-        <f t="shared" si="36"/>
+      <c r="D118" s="5">
+        <f t="shared" si="38"/>
         <v>2.76</v>
       </c>
-      <c r="E107" s="5">
-        <f t="shared" si="36"/>
+      <c r="E118" s="5">
+        <f t="shared" si="38"/>
         <v>3.9599999999999995</v>
       </c>
-      <c r="F107" s="5">
-        <f t="shared" si="36"/>
+      <c r="F118" s="5">
+        <f t="shared" si="38"/>
         <v>3.36</v>
       </c>
-      <c r="G107" s="5">
-        <f t="shared" si="36"/>
+      <c r="G118" s="5">
+        <f t="shared" si="38"/>
         <v>5.76</v>
       </c>
-      <c r="H107" s="5">
-        <f t="shared" si="36"/>
+      <c r="H118" s="5">
+        <f t="shared" si="38"/>
         <v>5.1599999999999993</v>
       </c>
-      <c r="I107" s="5">
-        <f t="shared" si="36"/>
+      <c r="I118" s="5">
+        <f t="shared" si="38"/>
         <v>0.96</v>
       </c>
-      <c r="J107" s="5">
-        <f t="shared" si="36"/>
+      <c r="J118" s="5">
+        <f t="shared" si="38"/>
         <v>2.16</v>
       </c>
-      <c r="K107" s="5">
-        <f t="shared" si="36"/>
+      <c r="K118" s="5">
+        <f t="shared" si="38"/>
         <v>1.56</v>
       </c>
-      <c r="L107" s="5">
-        <f t="shared" si="36"/>
+      <c r="L118" s="5">
+        <f t="shared" si="38"/>
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="108" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B108" t="s">
+    <row r="119" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
         <v>21</v>
       </c>
-      <c r="C108" s="5">
-        <f t="shared" ref="C108:L108" si="37">C75*C29</f>
+      <c r="C119" s="5">
+        <f t="shared" ref="C119:L119" si="39">C86*C29</f>
         <v>2.2200000000000002</v>
       </c>
-      <c r="D108" s="5">
-        <f t="shared" si="37"/>
+      <c r="D119" s="5">
+        <f t="shared" si="39"/>
         <v>3.42</v>
       </c>
-      <c r="E108" s="5">
-        <f t="shared" si="37"/>
+      <c r="E119" s="5">
+        <f t="shared" si="39"/>
         <v>6.419999999999999</v>
       </c>
-      <c r="F108" s="5">
-        <f t="shared" si="37"/>
+      <c r="F119" s="5">
+        <f t="shared" si="39"/>
         <v>1.02</v>
       </c>
-      <c r="G108" s="5">
-        <f t="shared" si="37"/>
+      <c r="G119" s="5">
+        <f t="shared" si="39"/>
         <v>5.8199999999999994</v>
       </c>
-      <c r="H108" s="5">
-        <f t="shared" si="37"/>
+      <c r="H119" s="5">
+        <f t="shared" si="39"/>
         <v>4.0199999999999996</v>
       </c>
-      <c r="I108" s="5">
-        <f t="shared" si="37"/>
+      <c r="I119" s="5">
+        <f t="shared" si="39"/>
         <v>4.62</v>
       </c>
-      <c r="J108" s="5">
-        <f t="shared" si="37"/>
+      <c r="J119" s="5">
+        <f t="shared" si="39"/>
         <v>5.22</v>
       </c>
-      <c r="K108" s="5">
-        <f t="shared" si="37"/>
+      <c r="K119" s="5">
+        <f t="shared" si="39"/>
         <v>1.62</v>
       </c>
-      <c r="L108" s="5">
-        <f t="shared" si="37"/>
+      <c r="L119" s="5">
+        <f t="shared" si="39"/>
         <v>2.82</v>
       </c>
     </row>
-    <row r="109" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
+    <row r="120" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
         <v>22</v>
       </c>
-      <c r="C109" s="5">
-        <f t="shared" ref="C109:L109" si="38">C76*C30</f>
+      <c r="C120" s="5">
+        <f t="shared" ref="C120:L120" si="40">C87*C30</f>
         <v>6.48</v>
       </c>
-      <c r="D109" s="5">
-        <f t="shared" si="38"/>
+      <c r="D120" s="5">
+        <f t="shared" si="40"/>
         <v>1.08</v>
       </c>
-      <c r="E109" s="5">
-        <f t="shared" si="38"/>
+      <c r="E120" s="5">
+        <f t="shared" si="40"/>
         <v>4.08</v>
       </c>
-      <c r="F109" s="5">
-        <f t="shared" si="38"/>
+      <c r="F120" s="5">
+        <f t="shared" si="40"/>
         <v>2.88</v>
       </c>
-      <c r="G109" s="5">
-        <f t="shared" si="38"/>
+      <c r="G120" s="5">
+        <f t="shared" si="40"/>
         <v>3.48</v>
       </c>
-      <c r="H109" s="5">
-        <f t="shared" si="38"/>
+      <c r="H120" s="5">
+        <f t="shared" si="40"/>
         <v>2.2799999999999998</v>
       </c>
-      <c r="I109" s="5">
-        <f t="shared" si="38"/>
+      <c r="I120" s="5">
+        <f t="shared" si="40"/>
         <v>4.68</v>
       </c>
-      <c r="J109" s="5">
-        <f t="shared" si="38"/>
+      <c r="J120" s="5">
+        <f t="shared" si="40"/>
         <v>5.28</v>
       </c>
-      <c r="K109" s="5">
-        <f t="shared" si="38"/>
+      <c r="K120" s="5">
+        <f t="shared" si="40"/>
         <v>1.68</v>
       </c>
-      <c r="L109" s="5">
-        <f t="shared" si="38"/>
-        <v>5.88</v>
-      </c>
-    </row>
-    <row r="110" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B110" t="s">
-        <v>23</v>
-      </c>
-      <c r="C110" s="5">
-        <f t="shared" ref="C110:L110" si="39">C77*C31</f>
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="D110" s="5">
-        <f t="shared" si="39"/>
-        <v>5.94</v>
-      </c>
-      <c r="E110" s="5">
-        <f t="shared" si="39"/>
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="F110" s="5">
-        <f t="shared" si="39"/>
-        <v>2.94</v>
-      </c>
-      <c r="G110" s="5">
-        <f t="shared" si="39"/>
-        <v>3.54</v>
-      </c>
-      <c r="H110" s="5">
-        <f t="shared" si="39"/>
-        <v>4.74</v>
-      </c>
-      <c r="I110" s="5">
-        <f t="shared" si="39"/>
-        <v>2.34</v>
-      </c>
-      <c r="J110" s="5">
-        <f t="shared" si="39"/>
-        <v>5.34</v>
-      </c>
-      <c r="K110" s="5">
-        <f t="shared" si="39"/>
-        <v>1.74</v>
-      </c>
-      <c r="L110" s="5">
-        <f t="shared" si="39"/>
-        <v>6.54</v>
-      </c>
-    </row>
-    <row r="111" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C111" s="5">
-        <f t="shared" ref="C111:L111" si="40">C78*C32</f>
-        <v>1.74</v>
-      </c>
-      <c r="D111" s="5">
-        <f t="shared" si="40"/>
-        <v>3.24</v>
-      </c>
-      <c r="E111" s="5">
+      <c r="L120" s="5">
         <f t="shared" si="40"/>
         <v>5.88</v>
       </c>
-      <c r="F111" s="5">
-        <f t="shared" si="40"/>
+    </row>
+    <row r="121" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121" s="5">
+        <f t="shared" ref="C121:L121" si="41">C88*C31</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D121" s="5">
+        <f t="shared" si="41"/>
+        <v>5.94</v>
+      </c>
+      <c r="E121" s="5">
+        <f t="shared" si="41"/>
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F121" s="5">
+        <f t="shared" si="41"/>
+        <v>2.94</v>
+      </c>
+      <c r="G121" s="5">
+        <f t="shared" si="41"/>
+        <v>3.54</v>
+      </c>
+      <c r="H121" s="5">
+        <f t="shared" si="41"/>
+        <v>4.74</v>
+      </c>
+      <c r="I121" s="5">
+        <f t="shared" si="41"/>
+        <v>2.34</v>
+      </c>
+      <c r="J121" s="5">
+        <f t="shared" si="41"/>
+        <v>5.34</v>
+      </c>
+      <c r="K121" s="5">
+        <f t="shared" si="41"/>
+        <v>1.74</v>
+      </c>
+      <c r="L121" s="5">
+        <f t="shared" si="41"/>
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>24</v>
+      </c>
+      <c r="C122" s="5">
+        <f t="shared" ref="C122:L122" si="42">C89*C32</f>
+        <v>1.74</v>
+      </c>
+      <c r="D122" s="5">
+        <f t="shared" si="42"/>
+        <v>3.24</v>
+      </c>
+      <c r="E122" s="5">
+        <f t="shared" si="42"/>
+        <v>5.88</v>
+      </c>
+      <c r="F122" s="5">
+        <f t="shared" si="42"/>
         <v>3.3</v>
       </c>
-      <c r="G111" s="5">
-        <f t="shared" si="40"/>
+      <c r="G122" s="5">
+        <f t="shared" si="42"/>
         <v>2.82</v>
       </c>
-      <c r="H111" s="5">
-        <f t="shared" si="40"/>
+      <c r="H122" s="5">
+        <f t="shared" si="42"/>
         <v>1.38</v>
       </c>
-      <c r="I111" s="5">
-        <f t="shared" si="40"/>
+      <c r="I122" s="5">
+        <f t="shared" si="42"/>
         <v>3.84</v>
       </c>
-      <c r="J111" s="5">
-        <f t="shared" si="40"/>
+      <c r="J122" s="5">
+        <f t="shared" si="42"/>
         <v>4.68</v>
       </c>
-      <c r="K111" s="5">
-        <f t="shared" si="40"/>
+      <c r="K122" s="5">
+        <f t="shared" si="42"/>
         <v>2.04</v>
       </c>
-      <c r="L111" s="5">
-        <f t="shared" si="40"/>
+      <c r="L122" s="5">
+        <f t="shared" si="42"/>
         <v>2.6999999999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+    <row r="125" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>51</v>
       </c>
-      <c r="C114" s="5">
-        <f>SUM(C89:L89) + SUM(C92:L111)</f>
+      <c r="C125" s="5">
+        <f>SUM(C100:L100) + SUM(C103:L122)</f>
         <v>1183.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Genetic Algorithm Now Features Grandchildren
Grandchildren help improved the breadth of search and increase the liklihood of discovering hard-to-reach solutions
</commit_message>
<xml_diff>
--- a/Excel/sample_fitness_calc.xlsx
+++ b/Excel/sample_fitness_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irawinder/Gits/GeneticAlgorithm/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2977724-DA5F-1F49-A8C0-3D9B830FC0A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10A5025-4B08-C74B-9DF7-C372CC299A0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17640" yWindow="3280" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>